<commit_message>
added meeting protocol and questions for tutor before mr1
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benni\Dropbox\Martin - Gabriel TU Wien\4. Semester\SEPM PR\Gruppenbeispiel\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,8 +16,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="1040" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -108,35 +108,38 @@
     <t>Punkte:</t>
   </si>
   <si>
-    <t>das war eig. Bis MR1 geplant:</t>
-  </si>
-  <si>
-    <t>Jetzt ca. ein Sprint bis zum MR 1</t>
-  </si>
-  <si>
-    <t>da wird voraussichtlich gemacht:</t>
-  </si>
-  <si>
-    <t>.) Kunde anlegen</t>
-  </si>
-  <si>
-    <t>.) Kunde bearbeiten (beides mit UI - nicht vergessen auf auslagern der Texte im UI)</t>
-  </si>
-  <si>
-    <t>.) Kunden-Demo-Demo-Daten erstellen</t>
-  </si>
-  <si>
-    <t>.) Demo-Daten für Veranstaltungen erstellen</t>
-  </si>
-  <si>
     <t>Mehrsprachigkeit - laufend</t>
+  </si>
+  <si>
+    <t>Storypoints pro Sprint:</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>Benni</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>1. Sprint bis hierher</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Verantwortlicher:</t>
+  </si>
+  <si>
+    <t>Christopher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +154,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -225,13 +236,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -244,17 +255,54 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -263,15 +311,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -282,6 +329,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -301,7 +371,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" diskRevisions="1" revisionId="72" version="21">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D940A152-4973-4D75-9614-BF1E9168855C}" diskRevisions="1" revisionId="98" version="32">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -403,6 +473,61 @@
     </sheetIdMap>
   </header>
   <header guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" dateTime="2017-04-22T12:27:24" maxSheetId="2" userName="Benni" r:id="rId21" minRId="72">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E04E7876-87D7-428C-9E7C-8C3ECFC0FB71}" dateTime="2017-04-24T21:11:20" maxSheetId="2" userName="Microsoft" r:id="rId22" minRId="73" maxRId="80">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{23638F32-B4DA-40C3-9A47-E667A1F818C4}" dateTime="2017-04-24T21:11:45" maxSheetId="2" userName="Microsoft" r:id="rId23" minRId="81" maxRId="82">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DD8DD0D0-EFBD-4761-B0FA-1800ACB3F902}" dateTime="2017-04-24T21:13:56" maxSheetId="2" userName="Microsoft" r:id="rId24">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4869E5F4-950E-425A-9F85-C486B4CACBAB}" dateTime="2017-04-24T21:16:16" maxSheetId="2" userName="Microsoft" r:id="rId25" minRId="83">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FF4CC62A-F7DE-48EA-998C-54581DC04D97}" dateTime="2017-04-24T21:22:57" maxSheetId="2" userName="Microsoft" r:id="rId26" minRId="84" maxRId="89">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F0D33547-2A3F-4C5E-AFE9-E47388F393EB}" dateTime="2017-04-24T21:23:14" maxSheetId="2" userName="Microsoft" r:id="rId27">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F43B1A8A-AF05-4510-B16C-8814B8211959}" dateTime="2017-04-24T21:24:19" maxSheetId="2" userName="Microsoft" r:id="rId28" minRId="90" maxRId="93">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0ECB1E76-7103-460E-BE6F-38C41B57772F}" dateTime="2017-04-24T21:26:17" maxSheetId="2" userName="Microsoft" r:id="rId29" minRId="94" maxRId="97">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4A6F4A86-D4ED-4EA4-8B51-6A32563769E8}" dateTime="2017-04-24T21:26:29" maxSheetId="2" userName="Microsoft" r:id="rId30">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{76A35DCA-5D1E-4E72-A3F3-5FD70A23A358}" dateTime="2017-04-24T21:26:44" maxSheetId="2" userName="Microsoft" r:id="rId31" minRId="98">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D940A152-4973-4D75-9614-BF1E9168855C}" dateTime="2017-04-24T21:26:47" maxSheetId="2" userName="Microsoft" r:id="rId32">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -633,6 +758,367 @@
       <v>4</v>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="73" sheetId="1" source="F14" destination="F16" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F16" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="74" sId="1">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>das war eig. Bis MR1 geplant:</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="75" sId="1">
+    <oc r="C35" t="inlineStr">
+      <is>
+        <t>Jetzt ca. ein Sprint bis zum MR 1</t>
+      </is>
+    </oc>
+    <nc r="C35"/>
+  </rcc>
+  <rcc rId="76" sId="1">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>da wird voraussichtlich gemacht:</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="77" sId="1">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>.) Kunde anlegen</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="78" sId="1">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>.) Kunde bearbeiten (beides mit UI - nicht vergessen auf auslagern der Texte im UI)</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="79" sId="1">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>.) Kunden-Demo-Demo-Daten erstellen</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="80" sId="1">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>.) Demo-Daten für Veranstaltungen erstellen</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="81" sId="1">
+    <nc r="F5" t="inlineStr">
+      <is>
+        <t>Storypoints pro Sprint:</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="82" sId="1">
+    <nc r="F6">
+      <v>40</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="F5:F6">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="F5" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F6" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F6">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="83" sId="1">
+    <oc r="F6">
+      <v>40</v>
+    </oc>
+    <nc r="F6">
+      <v>50</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="84" sheetId="1" source="F3" destination="F9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F9" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="85" sId="1">
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="86" sId="1">
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="87" sId="1">
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="88" sId="1">
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="89" sId="1">
+    <nc r="E8" t="inlineStr">
+      <is>
+        <t>Alex</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E5:E28">
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E28">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E28">
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E28">
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E28">
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:E14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="90" sId="1">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>1. Sprint bis hierher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="91" sheetId="1" source="B14" destination="A14" sourceSheetId="1"/>
+  <rcc rId="92" sId="1">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="93" sId="1">
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="94" sId="1">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <t>Verantwortlicher:</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="95" sId="1">
+    <nc r="E11" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="96" sId="1">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="97" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
 </revisions>
 </file>
 
@@ -807,6 +1293,130 @@
       </border>
     </dxf>
   </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E4" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D4" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E4" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="F5:F6" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5:F6" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F6" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F5" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rrc rId="98" sId="1" ref="F1:F1048576" action="insertCol"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
 </revisions>
@@ -1374,7 +1984,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" name="Microsoft Office-Anwender" id="-1182387524" dateTime="2017-04-22T12:05:17"/>
   <userInfo guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" name="Benni" id="-940673984" dateTime="2017-04-22T12:11:06"/>
@@ -1646,311 +2256,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="4"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="3"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="15">
         <v>2</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>8</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>8</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>8</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+      <c r="E13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="17">
         <v>4</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+      <c r="E14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="15">
         <v>5</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>1</v>
       </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="8" t="s">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>1</v>
       </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>6</v>
       </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="9">
+        <v>26</v>
+      </c>
+      <c r="D21" s="8">
         <v>5</v>
       </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
-      <c r="D22" s="11"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>4</v>
       </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>2</v>
       </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <v>10</v>
       </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <v>10</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>26</v>
-      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B40" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
+      <selection activeCell="G14" sqref="G14"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="B16" sqref="B16"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
proposal for new backlog and sprint planning
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" xWindow="355" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -133,13 +133,19 @@
   </si>
   <si>
     <t>Christopher</t>
+  </si>
+  <si>
+    <t>Veranstaltungen anzeigen</t>
+  </si>
+  <si>
+    <t>wären: 45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +164,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -324,12 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -344,15 +351,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -371,7 +392,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D940A152-4973-4D75-9614-BF1E9168855C}" diskRevisions="1" revisionId="98" version="32">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" diskRevisions="1" revisionId="111" version="36">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -528,6 +549,26 @@
     </sheetIdMap>
   </header>
   <header guid="{D940A152-4973-4D75-9614-BF1E9168855C}" dateTime="2017-04-24T21:26:47" maxSheetId="2" userName="Microsoft" r:id="rId32">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{66393CF5-0FDE-4512-8890-578A78AAC3E7}" dateTime="2017-04-29T13:17:41" maxSheetId="2" userName="Microsoft" r:id="rId33" minRId="99" maxRId="104">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{81D78350-56F2-4F79-8F34-9FA0C6006D6B}" dateTime="2017-04-29T13:17:53" maxSheetId="2" userName="Microsoft" r:id="rId34">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5BCC245A-D038-4ED2-846F-3E88B59B5762}" dateTime="2017-04-29T13:19:00" maxSheetId="2" userName="Microsoft" r:id="rId35" minRId="105" maxRId="110">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" dateTime="2017-04-29T13:19:09" maxSheetId="2" userName="Microsoft" r:id="rId36" minRId="111">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1419,6 +1460,256 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="99" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rrc rId="100" sId="1" ref="A8:XFD8" action="insertRow"/>
+  <rcc rId="101" sId="1">
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1">
+    <nc r="D8">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="1">
+    <oc r="D5">
+      <v>2</v>
+    </oc>
+    <nc r="D5">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="1">
+    <oc r="D6">
+      <v>2</v>
+    </oc>
+    <nc r="D6">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D5:D6 C8:D8" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="105" sheetId="1" source="C10:E10" destination="C34:E34" sourceSheetId="1"/>
+  <rrc rId="106" sId="1" ref="A10:XFD10" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A10:XFD10" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="107" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rm rId="108" sheetId="1" source="C34:E34" destination="C12:E12" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C12" start="0" length="0">
+      <dxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="109" sheetId="1" source="A15:B15" destination="A11:B11" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="C11:E11" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A11:B11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="110" sId="1">
+    <oc r="G6">
+      <v>50</v>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="111" sId="1">
+    <oc r="D9">
+      <v>20</v>
+    </oc>
+    <nc r="D9">
+      <v>24</v>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -2256,10 +2547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,10 +2566,10 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
@@ -2303,14 +2594,14 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15">
-        <v>2</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="22">
+        <v>4</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="20" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2319,15 +2610,15 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="23">
+        <v>3</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="19">
-        <v>50</v>
+      <c r="F6" s="11"/>
+      <c r="G6" s="21" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2337,37 +2628,35 @@
       <c r="D7" s="8">
         <v>8</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8">
-        <v>8</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13"/>
+      <c r="C8" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8">
-        <v>6</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="23">
+        <v>24</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -2376,233 +2665,243 @@
       <c r="D10" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="15">
         <v>4</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8">
-        <v>3</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="3"/>
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <v>8</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D15" s="8">
         <v>4</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D16" s="13">
         <v>5</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D17" s="8">
         <v>1</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D19" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" s="8">
-        <v>6</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8">
+        <v>6</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D22" s="8">
         <v>5</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="8">
-        <v>4</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D24" s="8">
-        <v>2</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D26" s="8">
-        <v>10</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="8">
         <v>10</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="8">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="8">
         <v>4</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
@@ -2615,11 +2914,14 @@
     </row>
     <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G19" sqref="G19"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>

</xml_diff>

<commit_message>
reworked product backlog with calvin, everything in red is new / reworked
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" xWindow="355" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -126,26 +126,48 @@
     <t>1. Sprint bis hierher</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
     <t>Verantwortlicher:</t>
   </si>
   <si>
     <t>Christopher</t>
   </si>
   <si>
-    <t>Veranstaltungen anzeigen</t>
-  </si>
-  <si>
-    <t>wären: 45</t>
+    <t>einzelne News anzeigen</t>
+  </si>
+  <si>
+    <t>News erstellen</t>
+  </si>
+  <si>
+    <t>gesehene News anzeigen/ausblenden</t>
+  </si>
+  <si>
+    <t>Veranstaltungen/Performances anzeigen</t>
+  </si>
+  <si>
+    <t>Verkauf von ausgewählten Ticktes</t>
+  </si>
+  <si>
+    <t>Customer selection in Saalplan</t>
+  </si>
+  <si>
+    <t>wären: 52</t>
+  </si>
+  <si>
+    <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+  </si>
+  <si>
+    <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +197,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -315,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -357,23 +398,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -392,7 +453,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" diskRevisions="1" revisionId="111" version="36">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{603823E5-CE07-4017-8D88-4645AD050333}" diskRevisions="1" revisionId="145" version="47">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -569,6 +630,61 @@
     </sheetIdMap>
   </header>
   <header guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" dateTime="2017-04-29T13:19:09" maxSheetId="2" userName="Microsoft" r:id="rId36" minRId="111">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C83FF58A-9A07-4F9A-9AC7-66EA08B9EB04}" dateTime="2017-04-29T17:39:28" maxSheetId="2" userName="Microsoft" r:id="rId37" minRId="112" maxRId="113">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B023F33C-AA89-488A-BBF9-02922DB5D2FA}" dateTime="2017-04-29T17:40:36" maxSheetId="2" userName="Microsoft" r:id="rId38" minRId="114" maxRId="119">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{75D88859-5FC7-4B07-8D78-F6D07ED55CFD}" dateTime="2017-04-29T17:41:43" maxSheetId="2" userName="Microsoft" r:id="rId39" minRId="120" maxRId="128">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{36D6F9EE-A4EF-4402-ADFB-2D1AF6D063AB}" dateTime="2017-04-29T17:42:05" maxSheetId="2" userName="Microsoft" r:id="rId40" minRId="129">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B16787EC-4036-4C68-A548-F79083FC9DCF}" dateTime="2017-04-29T17:44:27" maxSheetId="2" userName="Microsoft" r:id="rId41" minRId="130" maxRId="134">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5D044380-438D-45CC-BBA3-EB80158F26AA}" dateTime="2017-04-29T17:45:11" maxSheetId="2" userName="Microsoft" r:id="rId42" minRId="135" maxRId="138">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5C76CD5F-F0CF-4BA9-BB8B-425EAAE868E1}" dateTime="2017-04-29T17:45:58" maxSheetId="2" userName="Microsoft" r:id="rId43" minRId="139">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5F0E435C-195A-4E12-ABF6-24B398812027}" dateTime="2017-04-29T17:46:18" maxSheetId="2" userName="Microsoft" r:id="rId44" minRId="140">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{18EF123C-08DB-4690-B5AC-401D3A2BED42}" dateTime="2017-04-29T17:49:44" maxSheetId="2" userName="Microsoft" r:id="rId45" minRId="141">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{09C0619A-3ABD-48AF-81FF-EDEC2AC796BC}" dateTime="2017-04-29T17:50:18" maxSheetId="2" userName="Microsoft" r:id="rId46" minRId="142">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{603823E5-CE07-4017-8D88-4645AD050333}" dateTime="2017-04-29T17:51:09" maxSheetId="2" userName="Microsoft" r:id="rId47" minRId="143" maxRId="145">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1713,6 +1829,230 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="112" sId="1">
+    <oc r="D8">
+      <v>2</v>
+    </oc>
+    <nc r="D8">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="113" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="114" sId="1">
+    <oc r="D9">
+      <v>24</v>
+    </oc>
+    <nc r="D9">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="1">
+    <oc r="E14" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E14"/>
+  </rcc>
+  <rcc rId="116" sId="1">
+    <oc r="E15" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E15"/>
+  </rcc>
+  <rrc rId="117" sId="1" ref="A23:XFD23" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="118" sId="1">
+    <nc r="C23" t="inlineStr">
+      <is>
+        <t>einzelne News anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="1">
+    <nc r="D23">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C23:D23" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="120" sId="1" ref="A24:XFD24" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C24" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="121" sId="1" odxf="1" dxf="1">
+    <nc r="D24">
+      <v>3</v>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="122" sId="1">
+    <nc r="C24" t="inlineStr">
+      <is>
+        <t>News erstellen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="123" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="124" sId="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>gesehene News anzeigen/ausblenden</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="125" sheetId="1" source="C24:D24" destination="C35:D35" sourceSheetId="1"/>
+  <rm rId="126" sheetId="1" source="C23:D23" destination="C24:D24" sourceSheetId="1"/>
+  <rm rId="127" sheetId="1" source="C35:D35" destination="C23:D23" sourceSheetId="1"/>
+  <rcc rId="128" sId="1">
+    <nc r="D25">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rm rId="11" sheetId="1" source="C18" destination="C24" sourceSheetId="1">
@@ -1739,6 +2079,323 @@
   <rm rId="13" sheetId="1" source="C24" destination="C16" sourceSheetId="1"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="129" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C5:D6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog41.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="130" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen/Performances anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="131" sId="1" ref="A9:XFD9" action="insertRow"/>
+  <rm rId="132" sheetId="1" source="C10:E10" destination="C9:E9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E9" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcc rId="133" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Verkauf von ausgewählten Ticktes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="134" sId="1">
+    <nc r="D10">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog42.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="135" sId="1" ref="A10:XFD10" action="insertRow"/>
+  <rcc rId="136" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="137" sId="1">
+    <nc r="D10">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog43.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C10:G10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:G10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="139" sId="1" odxf="1" dxf="1">
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog44.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="140" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog45.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="141" sId="1">
+    <oc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E10"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog46.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="142" sId="1">
+    <oc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </oc>
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="143" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rcc rId="144" sId="1" odxf="1" dxf="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0" readingOrder="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="145" sId="1">
+    <nc r="D25">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C25:D25" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
 </revisions>
 </file>
 
@@ -2275,7 +2932,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" name="Microsoft Office-Anwender" id="-1182387524" dateTime="2017-04-22T12:05:17"/>
   <userInfo guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" name="Benni" id="-940673984" dateTime="2017-04-22T12:11:06"/>
@@ -2547,29 +3204,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
@@ -2584,17 +3241,17 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="26">
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -2607,18 +3264,18 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="27">
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="21" t="s">
-        <v>36</v>
+      <c r="G6" s="19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2635,11 +3292,11 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="23">
-        <v>2</v>
+      <c r="C8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="20">
+        <v>4</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2649,8 +3306,8 @@
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="23">
-        <v>24</v>
+      <c r="D9" s="20">
+        <v>20</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>30</v>
@@ -2658,131 +3315,128 @@
       <c r="F9" s="11"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+    <row r="10" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="30">
+        <v>2</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="28">
+        <v>3</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D12" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="E12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="14" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D13" s="15">
         <v>4</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="12" t="s">
+      <c r="E13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D14" s="13">
         <v>6</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8">
-        <v>3</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="8">
-        <v>8</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D15" s="8">
-        <v>4</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="18"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13">
-        <v>5</v>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="8">
+        <v>8</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="8">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="13">
+        <v>5</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="9">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8">
         <v>1</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
@@ -2791,137 +3445,203 @@
       <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="8">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D22" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
-      <c r="D23" s="10"/>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="8">
+        <v>6</v>
+      </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D24" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="8">
-        <v>2</v>
+    <row r="25" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="20">
+        <v>4</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="8">
-        <v>2</v>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="20">
+        <v>3</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="8">
-        <v>10</v>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="20">
+        <v>3</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="8">
-        <v>10</v>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="20">
+        <v>1</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="8">
-        <v>4</v>
-      </c>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="8">
+        <v>4</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="5"/>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="8">
+        <v>2</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="8">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="8">
+        <v>10</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="8">
+        <v>4</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>

</xml_diff>

<commit_message>
Small changes to product backlog
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
+    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
     <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -117,12 +113,6 @@
     <t>Calvin</t>
   </si>
   <si>
-    <t>Benni</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>1. Sprint bis hierher</t>
   </si>
   <si>
@@ -148,26 +138,29 @@
   </si>
   <si>
     <t>Customer selection in Saalplan</t>
-  </si>
-  <si>
-    <t>wären: 52</t>
-  </si>
-  <si>
-    <t>soll das überhaupt im selben
-Fenster wie Saalplan sein????
-eher zuerst Kunde auswählen,
-danach Saalplan</t>
   </si>
   <si>
     <t>Übersicht alles Rechnungen/Reservierungen
 Stornierungen und PDF neu drucken</t>
   </si>
+  <si>
+    <t>Alex / Benni</t>
+  </si>
+  <si>
+    <t>Platzierung: später überlegen</t>
+  </si>
+  <si>
+    <t>Reservierungen/Verkäufe anzeigen</t>
+  </si>
+  <si>
+    <t>wären: 56</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,7 +213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -406,12 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,9 +409,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -432,8 +427,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,7 +449,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{603823E5-CE07-4017-8D88-4645AD050333}" diskRevisions="1" revisionId="145" version="47">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" diskRevisions="1" revisionId="166" version="4">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -689,11 +685,39 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{01E1650E-2E16-4B9F-AC6F-690256DD718A}" dateTime="2017-04-30T14:48:59" maxSheetId="2" userName="Alex" r:id="rId48" minRId="146" maxRId="165">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{16014D3B-0EFA-4026-924D-8B091FF9FA05}" dateTime="2017-04-30T14:49:20" maxSheetId="2" userName="Alex" r:id="rId49">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CE36F0C9-B20E-47E7-8744-736AED355D2C}" dateTime="2017-04-30T14:49:46" maxSheetId="2" userName="Alex" r:id="rId50">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CC968181-75FD-4583-8D56-6CCAB2E56C0D}" dateTime="2017-04-30T14:51:39" maxSheetId="2" userName="Alex" r:id="rId51" minRId="166">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" dateTime="2017-04-30T14:51:40" maxSheetId="2" userName="Alex" r:id="rId52">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,6 +746,333 @@
 </file>
 
 <file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog110.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="146" sId="1">
+    <oc r="C7" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Veramstaöti</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="147" sheetId="1" source="C8" destination="C7" sourceSheetId="1">
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>Veramstaöti</t>
+        </is>
+      </nc>
+      <ndxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+  </rm>
+  <rm rId="148" sheetId="1" source="B8" destination="C8" sourceSheetId="1"/>
+  <rm rId="149" sheetId="1" source="D8" destination="F7" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F7" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="150" sheetId="1" source="D7" destination="D8" sourceSheetId="1"/>
+  <rm rId="151" sheetId="1" source="F7" destination="D7" sourceSheetId="1"/>
+  <rcc rId="152" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="153" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Alex</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C8" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C8">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="154" sheetId="1" source="C8" destination="I9" sourceSheetId="1"/>
+  <rcc rId="155" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8"/>
+  </rcc>
+  <rm rId="156" sheetId="1" source="C9:G10" destination="C8:G9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="D8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G8" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="157" sId="1">
+    <nc r="D10">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rcc rId="158" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10 D10 C10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="159" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </oc>
+    <nc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C9:G9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C9 D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rm rId="160" sheetId="1" source="C11:D11" destination="G12:H12" sourceSheetId="1"/>
+  <rm rId="161" sheetId="1" source="C12:E12" destination="C11:E11" sourceSheetId="1"/>
+  <rm rId="162" sheetId="1" source="G12:H12" destination="C12:D12" sourceSheetId="1"/>
+  <rrc rId="163" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rcc rId="164" sId="1">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Reservierungen/Verkäufe anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="165" sId="1">
+    <nc r="D12">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog1111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="53" sId="1">
     <nc r="D16">
@@ -749,6 +1100,25 @@
     </nc>
   </rcc>
   <rcv guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog112.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="166" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
 </revisions>
 </file>
 
@@ -776,6 +1146,13 @@
 </file>
 
 <file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog141.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="60" sId="1">
     <nc r="D7">
@@ -2932,13 +3309,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
-  <userInfo guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" name="Microsoft Office-Anwender" id="-1182387524" dateTime="2017-04-22T12:05:17"/>
-  <userInfo guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" name="Benni" id="-940673984" dateTime="2017-04-22T12:11:06"/>
-  <userInfo guid="{6E32143D-2DAC-4DA1-9C06-7DECE03B8640}" name="Microsoft Office-Anwender" id="-1182379380" dateTime="2017-04-22T12:25:45"/>
-  <userInfo guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" name="Microsoft Office-Anwender" id="-1182371220" dateTime="2017-04-22T12:28:01"/>
-</users>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2984,7 +3356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3019,7 +3391,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3196,21 +3568,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
@@ -3219,21 +3591,21 @@
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3241,17 +3613,17 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="B5" s="3"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="24">
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -3262,12 +3634,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="B6" s="3"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="25">
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -3275,168 +3647,165 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="8">
-        <v>8</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="20">
+        <v>4</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>39</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="21" t="s">
-        <v>37</v>
+    <row r="8" spans="1:9">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="20">
-        <v>4</v>
-      </c>
-      <c r="E8" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="20">
-        <v>20</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="29" t="s">
-        <v>39</v>
+    <row r="9" spans="1:9">
+      <c r="C9" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="34">
+        <v>2</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="C10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D10" s="30">
-        <v>2</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="28">
-        <v>3</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="8">
+    <row r="12" spans="1:9">
+      <c r="C12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="20">
         <v>4</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="26">
+        <v>3</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A14" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="15">
+        <v>4</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="15">
-        <v>4</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="12" t="s">
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D15" s="13">
         <v>6</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D16" s="8">
         <v>3</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="8">
-        <v>8</v>
-      </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="8">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="12" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D19" s="13">
         <v>5</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
@@ -3445,75 +3814,75 @@
       <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9">
+    <row r="21" spans="3:7">
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
         <v>1</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="8">
+    <row r="22" spans="3:7">
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9">
         <v>1</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D23" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D24" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C25" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="20">
-        <v>4</v>
+    <row r="25" spans="3:7">
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="8">
+        <v>5</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="21" t="s">
-        <v>35</v>
+    <row r="26" spans="3:7" ht="45">
+      <c r="C26" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="D26" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="C27" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="20">
         <v>3</v>
@@ -3522,49 +3891,49 @@
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7">
       <c r="C28" s="21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D28" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="10"/>
+    <row r="29" spans="3:7">
+      <c r="C29" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="8">
-        <v>4</v>
-      </c>
+    <row r="30" spans="3:7">
+      <c r="C30" s="3"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7">
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D31" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7">
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D32" s="8">
         <v>2</v>
@@ -3573,20 +3942,20 @@
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D33" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="C34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="8">
         <v>10</v>
@@ -3595,53 +3964,64 @@
       <c r="F34" s="11"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7">
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" thickBot="1">
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="8">
+        <v>4</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="43" spans="2:7" ht="15.75">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="2:7" ht="15.75">
       <c r="B44" s="5"/>
     </row>
-    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="15.75">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="15.75">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="15.75">
       <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:7" ht="15.75">
+      <c r="B48" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
+      <selection activeCell="G16" sqref="G16"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -3650,11 +4030,16 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
format product backlog and added me and calvin for one point
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
   </bookViews>
@@ -11,12 +16,12 @@
   </sheets>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
     <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
-    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
   </customWorkbookViews>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -155,12 +160,15 @@
   <si>
     <t>wären: 56</t>
   </si>
+  <si>
+    <t>Martin/Calvin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -324,15 +332,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -345,11 +344,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -379,19 +404,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -407,10 +426,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,17 +441,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -449,7 +479,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" diskRevisions="1" revisionId="166" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" diskRevisions="1" revisionId="167" version="6">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -706,6 +736,16 @@
     </sheetIdMap>
   </header>
   <header guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" dateTime="2017-04-30T14:51:40" maxSheetId="2" userName="Alex" r:id="rId52">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FD6FC766-CC2B-4CF6-8884-ED02F511E3A7}" dateTime="2017-05-01T18:48:28" maxSheetId="2" userName="Microsoft" r:id="rId53">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" dateTime="2017-05-01T18:48:47" maxSheetId="2" userName="Microsoft" r:id="rId54" minRId="167">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -2773,6 +2813,96 @@
       </font>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog48.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E8:E13" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I8:I13" start="0" length="0">
+    <dxf>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D7:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:E14" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E14:H14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:I15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D8:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog49.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="167" sId="1">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -3309,8 +3439,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3568,21 +3698,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
@@ -3591,10 +3721,10 @@
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3602,10 +3732,10 @@
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3618,43 +3748,43 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="18">
         <v>4</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -3662,103 +3792,127 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <v>20</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" s="33" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="27">
         <v>2</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="25">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="8">
         <v>4</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="C12" s="21" t="s">
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="18">
         <v>4</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" s="21" t="s">
+      <c r="E12" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="30">
         <v>3</v>
       </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A14" s="22" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="37">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="13">
         <v>6</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="F15" s="36"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
@@ -3771,7 +3925,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
@@ -3782,17 +3936,17 @@
       <c r="F17" s="11"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="3:7">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3803,7 +3957,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
@@ -3814,7 +3968,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3825,7 +3979,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
@@ -3836,7 +3990,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
@@ -3847,7 +4001,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
@@ -3858,7 +4012,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
@@ -3869,58 +4023,58 @@
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="3:7" ht="45">
-      <c r="C26" s="27" t="s">
+    <row r="26" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C26" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <v>4</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="3:7">
-      <c r="C27" s="21" t="s">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="18">
         <v>3</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="3:7">
-      <c r="C28" s="21" t="s">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="18">
         <v>3</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="3:7">
-      <c r="C29" s="21" t="s">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="18">
         <v>1</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="3:7">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="3:7">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
         <v>22</v>
       </c>
@@ -3931,7 +4085,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="3:7">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>24</v>
       </c>
@@ -3942,7 +4096,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
@@ -3953,7 +4107,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
@@ -3964,7 +4118,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
         <v>20</v>
       </c>
@@ -3975,7 +4129,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:7" ht="15.75" thickBot="1">
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="2" t="s">
         <v>21</v>
       </c>
@@ -3985,43 +4139,43 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="15.75" thickBot="1">
+    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="43" spans="2:7" ht="15.75">
+    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="2:7" ht="15.75">
+    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
     </row>
-    <row r="45" spans="2:7" ht="15.75">
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="2:7" ht="15.75">
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="15.75">
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="2:7" ht="15.75">
+    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
-      <selection activeCell="G16" sqref="G16"/>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -4030,8 +4184,8 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
+      <selection activeCell="G16" sqref="G16"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>

<commit_message>
added multi language support for all headlines of all tabs and updated Product Backlog after Tutor Meeting
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8390"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
     <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
+    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -64,9 +65,6 @@
     <t>Veranstaltungsarten</t>
   </si>
   <si>
-    <t>Saalplan</t>
-  </si>
-  <si>
     <t>Ticketverkauf</t>
   </si>
   <si>
@@ -140,9 +138,6 @@
   </si>
   <si>
     <t>Verkauf von ausgewählten Ticktes</t>
-  </si>
-  <si>
-    <t>Customer selection in Saalplan</t>
   </si>
   <si>
     <t>Übersicht alles Rechnungen/Reservierungen
@@ -152,23 +147,38 @@
     <t>Alex / Benni</t>
   </si>
   <si>
-    <t>Platzierung: später überlegen</t>
-  </si>
-  <si>
     <t>Reservierungen/Verkäufe anzeigen</t>
   </si>
   <si>
-    <t>wären: 56</t>
-  </si>
-  <si>
     <t>Martin/Calvin</t>
+  </si>
+  <si>
+    <t>Customer selection nach Saalplan</t>
+  </si>
+  <si>
+    <t>Martin/Christopher</t>
+  </si>
+  <si>
+    <t>(Alex / Benni) Calvin?</t>
+  </si>
+  <si>
+    <t>Saalplan Sitzplätze</t>
+  </si>
+  <si>
+    <t>Saalplan Sektoren</t>
+  </si>
+  <si>
+    <t>wären: 47</t>
+  </si>
+  <si>
+    <t>vllt noch in erstem Sprint?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,13 +203,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +228,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -317,21 +326,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -344,37 +338,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -403,37 +371,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,25 +422,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,7 +448,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" diskRevisions="1" revisionId="167" version="6">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7C64980B-A064-4084-8801-1814945BDF5E}" diskRevisions="1" revisionId="185" version="13">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -746,6 +715,41 @@
     </sheetIdMap>
   </header>
   <header guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" dateTime="2017-05-01T18:48:47" maxSheetId="2" userName="Microsoft" r:id="rId54" minRId="167">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A133C022-AFE6-447E-BECA-8B93C5221737}" dateTime="2017-05-03T16:06:28" maxSheetId="2" userName="Martin Klampfer" r:id="rId55" minRId="168" maxRId="176">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{889BB63A-29AE-4B6E-85A4-F158D5946810}" dateTime="2017-05-03T16:06:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId56" minRId="177" maxRId="178">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{19038F75-9BEF-4375-9595-4ED078EB4966}" dateTime="2017-05-03T16:08:34" maxSheetId="2" userName="Martin Klampfer" r:id="rId57" minRId="179" maxRId="184">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6AF878D6-9310-4021-BBDE-8E4786BC598C}" dateTime="2017-05-03T16:08:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId58">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{566CAB0B-B727-4D41-8831-C2010EC0A46F}" dateTime="2017-05-03T16:09:49" maxSheetId="2" userName="Martin Klampfer" r:id="rId59" minRId="185">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9A2E6002-35E9-4C02-A72A-3D5A8BF0E06C}" dateTime="2017-05-03T16:09:56" maxSheetId="2" userName="Martin Klampfer" r:id="rId60">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7C64980B-A064-4084-8801-1814945BDF5E}" dateTime="2017-05-03T16:10:00" maxSheetId="2" userName="Martin Klampfer" r:id="rId61">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -3178,6 +3182,299 @@
   </rfmt>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog50.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="168" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </oc>
+    <nc r="G9"/>
+  </rcc>
+  <rm rId="169" sheetId="1" source="A14:B14" destination="A12:B12" sourceSheetId="1"/>
+  <rcc rId="170" sId="1">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection nach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="A7:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C7:D18" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="171" sId="1">
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="172" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="173" sheetId="1" source="C13:D13" destination="C39:D39" sourceSheetId="1"/>
+  <rm rId="174" sheetId="1" source="C14:E14" destination="C13:E13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E13" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rm rId="175" sheetId="1" source="C39:D39" destination="C14:D14" sourceSheetId="1"/>
+  <rm rId="176" sheetId="1" source="A12" destination="A13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="A13" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="177" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="178" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog52.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="179" sheetId="1" source="A14:F37" destination="A15:F38" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="180" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Saalplan Sitzplätze</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="181" sId="1">
+    <nc r="D14">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="182" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan Sektoren</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="183" sId="1">
+    <oc r="D8">
+      <v>20</v>
+    </oc>
+    <nc r="D8">
+      <v>14</v>
+    </nc>
+  </rcc>
+  <rcc rId="184" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="delete"/>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog53.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C27:D30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog54.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="185" sId="1">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>vllt noch in erstem Sprint?</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog55.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14:D17" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog56.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D10:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
 </revisions>
 </file>
 
@@ -3439,7 +3736,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -3486,7 +3783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3521,7 +3818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3709,268 +4006,281 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="3"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="31" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="21" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="28">
         <v>4</v>
       </c>
-      <c r="D6" s="23">
-        <v>3</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="17" t="s">
+      <c r="E7" s="11" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="18">
-        <v>4</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="28">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="29">
+        <v>2</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="18">
-        <v>20</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
+      <c r="D10" s="30">
+        <v>8</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="27">
-        <v>2</v>
-      </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="28">
+        <v>4</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="25">
-        <v>8</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="28">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="8">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28">
         <v>4</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
+      <c r="E13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="18">
-        <v>4</v>
-      </c>
-      <c r="E12" s="31" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C14" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
+      <c r="D14" s="28">
+        <v>10</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="23"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="30">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="38">
         <v>3</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
+      <c r="E15" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="14" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="37">
-        <v>4</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="13">
+      <c r="D16" s="28">
         <v>6</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8">
-        <v>3</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="11"/>
+      <c r="E16" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="24"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="8">
-        <v>8</v>
-      </c>
-      <c r="E17" s="11"/>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="28">
+        <v>3</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="8">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="28">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="28">
         <v>4</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="13">
-        <v>5</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13">
+        <v>5</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
@@ -3979,124 +4289,124 @@
       <c r="F21" s="11"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="9">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="8">
         <v>1</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="8">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="9">
         <v>1</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D24" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D25" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C26" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="18">
-        <v>4</v>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="8">
+        <v>5</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="18">
-        <v>3</v>
+    <row r="27" spans="3:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="28">
+        <v>4</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="19" t="s">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="28">
         <v>3</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="18">
-        <v>1</v>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="28">
+        <v>3</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
-      <c r="D30" s="10"/>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="28">
+        <v>1</v>
+      </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="8">
-        <v>4</v>
-      </c>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D32" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
@@ -4107,20 +4417,20 @@
       <c r="F33" s="11"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D34" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D35" s="8">
         <v>10</v>
@@ -4129,47 +4439,53 @@
       <c r="F35" s="11"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D36" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="8">
+        <v>4</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B44" s="5"/>
     </row>
-    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B48" s="5"/>
     </row>
   </sheetData>
@@ -4189,11 +4505,16 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated erd and product backlog incl sprint planning
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="1135" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
-    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>Veranstaltungsarten</t>
-  </si>
-  <si>
-    <t>Ticketverkauf</t>
-  </si>
-  <si>
-    <t>Ticketreservierungen</t>
   </si>
   <si>
     <t>Stornierung von Ticketreservierungen</t>
@@ -150,16 +144,7 @@
     <t>Reservierungen/Verkäufe anzeigen</t>
   </si>
   <si>
-    <t>Martin/Calvin</t>
-  </si>
-  <si>
     <t>Customer selection nach Saalplan</t>
-  </si>
-  <si>
-    <t>Martin/Christopher</t>
-  </si>
-  <si>
-    <t>(Alex / Benni) Calvin?</t>
   </si>
   <si>
     <t>Saalplan Sitzplätze</t>
@@ -168,17 +153,53 @@
     <t>Saalplan Sektoren</t>
   </si>
   <si>
-    <t>wären: 47</t>
+    <t>vllt noch in erstem Sprint?</t>
   </si>
   <si>
-    <t>vllt noch in erstem Sprint?</t>
+    <t>Martin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Martin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Calvin</t>
+    </r>
+  </si>
+  <si>
+    <t>Ticketverkauf, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketverkauf, serverseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, serverseitig</t>
+  </si>
+  <si>
+    <t>Christopher, Calvin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +235,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,14 +270,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -338,11 +374,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -422,13 +473,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,7 +518,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7C64980B-A064-4084-8801-1814945BDF5E}" diskRevisions="1" revisionId="185" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{50242816-3825-4FDE-8AC5-9767A747207A}" diskRevisions="1" revisionId="211" version="19">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -750,6 +820,36 @@
     </sheetIdMap>
   </header>
   <header guid="{7C64980B-A064-4084-8801-1814945BDF5E}" dateTime="2017-05-03T16:10:00" maxSheetId="2" userName="Martin Klampfer" r:id="rId61">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{874C0D29-8150-4D0C-9A0D-8ED1CF64EE82}" dateTime="2017-05-07T17:09:01" maxSheetId="2" userName="Microsoft" r:id="rId62" minRId="186" maxRId="188">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3F184119-29BE-43A1-AEDE-BB639519E443}" dateTime="2017-05-07T17:09:09" maxSheetId="2" userName="Microsoft" r:id="rId63" minRId="189">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6591666E-586B-444E-9942-3D0D6E6B6951}" dateTime="2017-05-07T17:09:19" maxSheetId="2" userName="Microsoft" r:id="rId64">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2C4B1529-DFDB-46F2-B2FF-B354077682B9}" dateTime="2017-05-07T17:13:28" maxSheetId="2" userName="Microsoft" r:id="rId65" minRId="190" maxRId="193">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1292FC90-6409-4788-AE41-4BD648128DC5}" dateTime="2017-05-07T17:14:59" maxSheetId="2" userName="Microsoft" r:id="rId66" minRId="194" maxRId="210">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{50242816-3825-4FDE-8AC5-9767A747207A}" dateTime="2017-05-07T17:26:12" maxSheetId="2" userName="Microsoft" r:id="rId67" minRId="211">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -3478,6 +3578,165 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog57.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="186" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="187" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="188" sheetId="1" source="A13" destination="A12" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="E13" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15:E17" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog58.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="189" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog59.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rfmt sheetId="1" sqref="C22" start="0" length="0">
@@ -3553,6 +3812,461 @@
       </border>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog60.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="190" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="191" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="192" sheetId="1" source="E10" destination="F10" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="193" sId="1" odxf="1" dxf="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:F11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog61.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="194" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rm rId="195" sheetId="1" source="C13:D13" destination="C14:D14" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D13:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D14">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rrc rId="196" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C13" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="197" sId="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="198" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="199" sId="1">
+    <oc r="D10">
+      <v>8</v>
+    </oc>
+    <nc r="D10">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="200" sId="1">
+    <oc r="D11">
+      <v>4</v>
+    </oc>
+    <nc r="D11">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="201" sId="1">
+    <oc r="E13" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </oc>
+    <nc r="E13"/>
+  </rcc>
+  <rcc rId="202" sId="1" odxf="1" dxf="1">
+    <nc r="D13">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="203" sId="1" odxf="1" dxf="1">
+    <nc r="D14">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="204" sId="1">
+    <oc r="F10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F10"/>
+  </rcc>
+  <rcc rId="205" sId="1">
+    <oc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F11"/>
+  </rcc>
+  <rcc rId="206" sId="1">
+    <oc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="207" sId="1">
+    <oc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen</t>
+      </is>
+    </oc>
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="208" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:E11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="0">
+    <dxf>
+      <alignment horizontal="left" vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="209" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher, Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="210" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog62.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="211" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </oc>
+    <nc r="G6">
+      <v>40</v>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -4003,25 +4717,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
@@ -4029,23 +4743,23 @@
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="16" t="s">
         <v>3</v>
@@ -4053,15 +4767,15 @@
       <c r="D5" s="17">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>27</v>
+      <c r="E5" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="16" t="s">
         <v>4</v>
@@ -4069,103 +4783,108 @@
       <c r="D6" s="18">
         <v>3</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>27</v>
+      <c r="E6" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="31" t="s">
-        <v>45</v>
+      <c r="G6" s="31">
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="28">
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="18">
         <v>4</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>42</v>
+      <c r="E7" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D8" s="28">
         <v>14</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="29">
         <v>2</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="26" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D10" s="30">
-        <v>8</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+        <v>4</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="45"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="26" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D11" s="28">
-        <v>4</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="19"/>
+        <v>3</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="45"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>26</v>
+      </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="28">
+      <c r="C12" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="43">
         <v>4</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="44" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="19"/>
@@ -4173,147 +4892,148 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
-        <v>28</v>
-      </c>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="25"/>
       <c r="C13" s="26" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D13" s="28">
-        <v>4</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>30</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E13" s="36"/>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="28">
-        <v>10</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="23"/>
+      <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
-      <c r="C15" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="38">
+      <c r="C15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="28">
+        <v>4</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="28">
+        <v>10</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="40">
         <v>3</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="E17" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="28">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="28">
         <v>6</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="3"/>
+      <c r="E18" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="3"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="28">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="28">
         <v>3</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="28">
-        <v>8</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="28">
-        <v>4</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C20" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13">
-        <v>5</v>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="28">
+        <v>8</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="28">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="8">
         <v>1</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -4322,181 +5042,203 @@
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="8">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D26" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="3:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="C27" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="28">
-        <v>4</v>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="8">
+        <v>6</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="28">
-        <v>3</v>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="8">
+        <v>5</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C29" s="26" t="s">
-        <v>31</v>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="D29" s="28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C31" s="3"/>
-      <c r="D31" s="10"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="28">
+        <v>3</v>
+      </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="8">
-        <v>4</v>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="28">
+        <v>1</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="8">
-        <v>2</v>
-      </c>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D34" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D35" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D36" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
+      <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D37" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
+      <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="1" t="s">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="8">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="3"/>
+      <c r="G40" s="3"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="6"/>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="6"/>
     </row>
-    <row r="43" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C43" s="5"/>
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
     </row>
-    <row r="44" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B44" s="5"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="5"/>
-    </row>
-    <row r="46" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G11" sqref="G11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -4505,8 +5247,8 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
-      <selection activeCell="G7" sqref="G7"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>

</xml_diff>

<commit_message>
updated erd and product backlog
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="1135" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -61,15 +63,6 @@
   </si>
   <si>
     <t>Veranstaltungsarten</t>
-  </si>
-  <si>
-    <t>Saalplan</t>
-  </si>
-  <si>
-    <t>Ticketverkauf</t>
-  </si>
-  <si>
-    <t>Ticketreservierungen</t>
   </si>
   <si>
     <t>Stornierung von Ticketreservierungen</t>
@@ -117,16 +110,7 @@
     <t>Calvin</t>
   </si>
   <si>
-    <t>Benni</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>1. Sprint bis hierher</t>
-  </si>
-  <si>
-    <t>Martin</t>
   </si>
   <si>
     <t>Verantwortlicher:</t>
@@ -134,12 +118,88 @@
   <si>
     <t>Christopher</t>
   </si>
+  <si>
+    <t>einzelne News anzeigen</t>
+  </si>
+  <si>
+    <t>News erstellen</t>
+  </si>
+  <si>
+    <t>gesehene News anzeigen/ausblenden</t>
+  </si>
+  <si>
+    <t>Veranstaltungen/Performances anzeigen</t>
+  </si>
+  <si>
+    <t>Verkauf von ausgewählten Ticktes</t>
+  </si>
+  <si>
+    <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+  </si>
+  <si>
+    <t>Alex / Benni</t>
+  </si>
+  <si>
+    <t>Reservierungen/Verkäufe anzeigen</t>
+  </si>
+  <si>
+    <t>Customer selection nach Saalplan</t>
+  </si>
+  <si>
+    <t>Saalplan Sitzplätze</t>
+  </si>
+  <si>
+    <t>Saalplan Sektoren</t>
+  </si>
+  <si>
+    <t>vllt noch in erstem Sprint?</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Martin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Calvin</t>
+    </r>
+  </si>
+  <si>
+    <t>Ticketverkauf, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketverkauf, serverseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, serverseitig</t>
+  </si>
+  <si>
+    <t>Christopher, Calvin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +222,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -262,6 +362,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -276,33 +389,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -324,12 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -337,20 +422,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -371,7 +518,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D940A152-4973-4D75-9614-BF1E9168855C}" diskRevisions="1" revisionId="98" version="32">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{50242816-3825-4FDE-8AC5-9767A747207A}" diskRevisions="1" revisionId="211" version="19">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -532,11 +679,189 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{66393CF5-0FDE-4512-8890-578A78AAC3E7}" dateTime="2017-04-29T13:17:41" maxSheetId="2" userName="Microsoft" r:id="rId33" minRId="99" maxRId="104">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{81D78350-56F2-4F79-8F34-9FA0C6006D6B}" dateTime="2017-04-29T13:17:53" maxSheetId="2" userName="Microsoft" r:id="rId34">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5BCC245A-D038-4ED2-846F-3E88B59B5762}" dateTime="2017-04-29T13:19:00" maxSheetId="2" userName="Microsoft" r:id="rId35" minRId="105" maxRId="110">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" dateTime="2017-04-29T13:19:09" maxSheetId="2" userName="Microsoft" r:id="rId36" minRId="111">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C83FF58A-9A07-4F9A-9AC7-66EA08B9EB04}" dateTime="2017-04-29T17:39:28" maxSheetId="2" userName="Microsoft" r:id="rId37" minRId="112" maxRId="113">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B023F33C-AA89-488A-BBF9-02922DB5D2FA}" dateTime="2017-04-29T17:40:36" maxSheetId="2" userName="Microsoft" r:id="rId38" minRId="114" maxRId="119">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{75D88859-5FC7-4B07-8D78-F6D07ED55CFD}" dateTime="2017-04-29T17:41:43" maxSheetId="2" userName="Microsoft" r:id="rId39" minRId="120" maxRId="128">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{36D6F9EE-A4EF-4402-ADFB-2D1AF6D063AB}" dateTime="2017-04-29T17:42:05" maxSheetId="2" userName="Microsoft" r:id="rId40" minRId="129">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B16787EC-4036-4C68-A548-F79083FC9DCF}" dateTime="2017-04-29T17:44:27" maxSheetId="2" userName="Microsoft" r:id="rId41" minRId="130" maxRId="134">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5D044380-438D-45CC-BBA3-EB80158F26AA}" dateTime="2017-04-29T17:45:11" maxSheetId="2" userName="Microsoft" r:id="rId42" minRId="135" maxRId="138">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5C76CD5F-F0CF-4BA9-BB8B-425EAAE868E1}" dateTime="2017-04-29T17:45:58" maxSheetId="2" userName="Microsoft" r:id="rId43" minRId="139">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5F0E435C-195A-4E12-ABF6-24B398812027}" dateTime="2017-04-29T17:46:18" maxSheetId="2" userName="Microsoft" r:id="rId44" minRId="140">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{18EF123C-08DB-4690-B5AC-401D3A2BED42}" dateTime="2017-04-29T17:49:44" maxSheetId="2" userName="Microsoft" r:id="rId45" minRId="141">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{09C0619A-3ABD-48AF-81FF-EDEC2AC796BC}" dateTime="2017-04-29T17:50:18" maxSheetId="2" userName="Microsoft" r:id="rId46" minRId="142">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{603823E5-CE07-4017-8D88-4645AD050333}" dateTime="2017-04-29T17:51:09" maxSheetId="2" userName="Microsoft" r:id="rId47" minRId="143" maxRId="145">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{01E1650E-2E16-4B9F-AC6F-690256DD718A}" dateTime="2017-04-30T14:48:59" maxSheetId="2" userName="Alex" r:id="rId48" minRId="146" maxRId="165">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{16014D3B-0EFA-4026-924D-8B091FF9FA05}" dateTime="2017-04-30T14:49:20" maxSheetId="2" userName="Alex" r:id="rId49">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CE36F0C9-B20E-47E7-8744-736AED355D2C}" dateTime="2017-04-30T14:49:46" maxSheetId="2" userName="Alex" r:id="rId50">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CC968181-75FD-4583-8D56-6CCAB2E56C0D}" dateTime="2017-04-30T14:51:39" maxSheetId="2" userName="Alex" r:id="rId51" minRId="166">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" dateTime="2017-04-30T14:51:40" maxSheetId="2" userName="Alex" r:id="rId52">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FD6FC766-CC2B-4CF6-8884-ED02F511E3A7}" dateTime="2017-05-01T18:48:28" maxSheetId="2" userName="Microsoft" r:id="rId53">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" dateTime="2017-05-01T18:48:47" maxSheetId="2" userName="Microsoft" r:id="rId54" minRId="167">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A133C022-AFE6-447E-BECA-8B93C5221737}" dateTime="2017-05-03T16:06:28" maxSheetId="2" userName="Martin Klampfer" r:id="rId55" minRId="168" maxRId="176">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{889BB63A-29AE-4B6E-85A4-F158D5946810}" dateTime="2017-05-03T16:06:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId56" minRId="177" maxRId="178">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{19038F75-9BEF-4375-9595-4ED078EB4966}" dateTime="2017-05-03T16:08:34" maxSheetId="2" userName="Martin Klampfer" r:id="rId57" minRId="179" maxRId="184">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6AF878D6-9310-4021-BBDE-8E4786BC598C}" dateTime="2017-05-03T16:08:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId58">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{566CAB0B-B727-4D41-8831-C2010EC0A46F}" dateTime="2017-05-03T16:09:49" maxSheetId="2" userName="Martin Klampfer" r:id="rId59" minRId="185">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9A2E6002-35E9-4C02-A72A-3D5A8BF0E06C}" dateTime="2017-05-03T16:09:56" maxSheetId="2" userName="Martin Klampfer" r:id="rId60">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7C64980B-A064-4084-8801-1814945BDF5E}" dateTime="2017-05-03T16:10:00" maxSheetId="2" userName="Martin Klampfer" r:id="rId61">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{874C0D29-8150-4D0C-9A0D-8ED1CF64EE82}" dateTime="2017-05-07T17:09:01" maxSheetId="2" userName="Microsoft" r:id="rId62" minRId="186" maxRId="188">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3F184119-29BE-43A1-AEDE-BB639519E443}" dateTime="2017-05-07T17:09:09" maxSheetId="2" userName="Microsoft" r:id="rId63" minRId="189">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6591666E-586B-444E-9942-3D0D6E6B6951}" dateTime="2017-05-07T17:09:19" maxSheetId="2" userName="Microsoft" r:id="rId64">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2C4B1529-DFDB-46F2-B2FF-B354077682B9}" dateTime="2017-05-07T17:13:28" maxSheetId="2" userName="Microsoft" r:id="rId65" minRId="190" maxRId="193">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1292FC90-6409-4788-AE41-4BD648128DC5}" dateTime="2017-05-07T17:14:59" maxSheetId="2" userName="Microsoft" r:id="rId66" minRId="194" maxRId="210">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{50242816-3825-4FDE-8AC5-9767A747207A}" dateTime="2017-05-07T17:26:12" maxSheetId="2" userName="Microsoft" r:id="rId67" minRId="211">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -565,6 +890,333 @@
 </file>
 
 <file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog110.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="146" sId="1">
+    <oc r="C7" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Veramstaöti</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="147" sheetId="1" source="C8" destination="C7" sourceSheetId="1">
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>Veramstaöti</t>
+        </is>
+      </nc>
+      <ndxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+  </rm>
+  <rm rId="148" sheetId="1" source="B8" destination="C8" sourceSheetId="1"/>
+  <rm rId="149" sheetId="1" source="D8" destination="F7" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F7" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="150" sheetId="1" source="D7" destination="D8" sourceSheetId="1"/>
+  <rm rId="151" sheetId="1" source="F7" destination="D7" sourceSheetId="1"/>
+  <rcc rId="152" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="153" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Alex</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C8" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C8">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="154" sheetId="1" source="C8" destination="I9" sourceSheetId="1"/>
+  <rcc rId="155" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8"/>
+  </rcc>
+  <rm rId="156" sheetId="1" source="C9:G10" destination="C8:G9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="D8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G8" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="157" sId="1">
+    <nc r="D10">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rcc rId="158" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10 D10 C10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="159" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </oc>
+    <nc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C9:G9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C9 D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rm rId="160" sheetId="1" source="C11:D11" destination="G12:H12" sourceSheetId="1"/>
+  <rm rId="161" sheetId="1" source="C12:E12" destination="C11:E11" sourceSheetId="1"/>
+  <rm rId="162" sheetId="1" source="G12:H12" destination="C12:D12" sourceSheetId="1"/>
+  <rrc rId="163" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rcc rId="164" sId="1">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Reservierungen/Verkäufe anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="165" sId="1">
+    <nc r="D12">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog1111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="53" sId="1">
     <nc r="D16">
@@ -595,6 +1247,25 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog112.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="166" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="1">
@@ -619,6 +1290,13 @@
 </file>
 
 <file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog141.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="60" sId="1">
     <nc r="D7">
@@ -1422,6 +2100,480 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="99" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rrc rId="100" sId="1" ref="A8:XFD8" action="insertRow"/>
+  <rcc rId="101" sId="1">
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1">
+    <nc r="D8">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="1">
+    <oc r="D5">
+      <v>2</v>
+    </oc>
+    <nc r="D5">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="1">
+    <oc r="D6">
+      <v>2</v>
+    </oc>
+    <nc r="D6">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D5:D6 C8:D8" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="105" sheetId="1" source="C10:E10" destination="C34:E34" sourceSheetId="1"/>
+  <rrc rId="106" sId="1" ref="A10:XFD10" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A10:XFD10" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="107" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rm rId="108" sheetId="1" source="C34:E34" destination="C12:E12" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C12" start="0" length="0">
+      <dxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="109" sheetId="1" source="A15:B15" destination="A11:B11" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="C11:E11" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A11:B11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="110" sId="1">
+    <oc r="G6">
+      <v>50</v>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="111" sId="1">
+    <oc r="D9">
+      <v>20</v>
+    </oc>
+    <nc r="D9">
+      <v>24</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="112" sId="1">
+    <oc r="D8">
+      <v>2</v>
+    </oc>
+    <nc r="D8">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="113" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="114" sId="1">
+    <oc r="D9">
+      <v>24</v>
+    </oc>
+    <nc r="D9">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="1">
+    <oc r="E14" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E14"/>
+  </rcc>
+  <rcc rId="116" sId="1">
+    <oc r="E15" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E15"/>
+  </rcc>
+  <rrc rId="117" sId="1" ref="A23:XFD23" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="118" sId="1">
+    <nc r="C23" t="inlineStr">
+      <is>
+        <t>einzelne News anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="1">
+    <nc r="D23">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C23:D23" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="120" sId="1" ref="A24:XFD24" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C24" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="121" sId="1" odxf="1" dxf="1">
+    <nc r="D24">
+      <v>3</v>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="122" sId="1">
+    <nc r="C24" t="inlineStr">
+      <is>
+        <t>News erstellen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="123" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="124" sId="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>gesehene News anzeigen/ausblenden</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="125" sheetId="1" source="C24:D24" destination="C35:D35" sourceSheetId="1"/>
+  <rm rId="126" sheetId="1" source="C23:D23" destination="C24:D24" sourceSheetId="1"/>
+  <rm rId="127" sheetId="1" source="C35:D35" destination="C23:D23" sourceSheetId="1"/>
+  <rcc rId="128" sId="1">
+    <nc r="D25">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rm rId="11" sheetId="1" source="C18" destination="C24" sourceSheetId="1">
@@ -1448,6 +2600,413 @@
   <rm rId="13" sheetId="1" source="C24" destination="C16" sourceSheetId="1"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="129" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C5:D6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog41.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="130" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen/Performances anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="131" sId="1" ref="A9:XFD9" action="insertRow"/>
+  <rm rId="132" sheetId="1" source="C10:E10" destination="C9:E9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E9" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcc rId="133" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Verkauf von ausgewählten Ticktes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="134" sId="1">
+    <nc r="D10">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog42.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="135" sId="1" ref="A10:XFD10" action="insertRow"/>
+  <rcc rId="136" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="137" sId="1">
+    <nc r="D10">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog43.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C10:G10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:G10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="139" sId="1" odxf="1" dxf="1">
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog44.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="140" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog45.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="141" sId="1">
+    <oc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E10"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog46.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="142" sId="1">
+    <oc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </oc>
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="143" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rcc rId="144" sId="1" odxf="1" dxf="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0" readingOrder="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="145" sId="1">
+    <nc r="D25">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C25:D25" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog48.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E8:E13" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I8:I13" start="0" length="0">
+    <dxf>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D7:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:E14" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E14:H14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:I15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D8:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog49.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="167" sId="1">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -1726,6 +3285,458 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog50.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="168" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </oc>
+    <nc r="G9"/>
+  </rcc>
+  <rm rId="169" sheetId="1" source="A14:B14" destination="A12:B12" sourceSheetId="1"/>
+  <rcc rId="170" sId="1">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection nach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="A7:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C7:D18" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="171" sId="1">
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="172" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="173" sheetId="1" source="C13:D13" destination="C39:D39" sourceSheetId="1"/>
+  <rm rId="174" sheetId="1" source="C14:E14" destination="C13:E13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E13" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rm rId="175" sheetId="1" source="C39:D39" destination="C14:D14" sourceSheetId="1"/>
+  <rm rId="176" sheetId="1" source="A12" destination="A13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="A13" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="177" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="178" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog52.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="179" sheetId="1" source="A14:F37" destination="A15:F38" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="180" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Saalplan Sitzplätze</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="181" sId="1">
+    <nc r="D14">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="182" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan Sektoren</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="183" sId="1">
+    <oc r="D8">
+      <v>20</v>
+    </oc>
+    <nc r="D8">
+      <v>14</v>
+    </nc>
+  </rcc>
+  <rcc rId="184" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="delete"/>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog53.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C27:D30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog54.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="185" sId="1">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>vllt noch in erstem Sprint?</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog55.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14:D17" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog56.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D10:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog57.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="186" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="187" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="188" sheetId="1" source="A13" destination="A12" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="E13" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15:E17" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog58.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="189" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog59.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rfmt sheetId="1" sqref="C22" start="0" length="0">
@@ -1801,6 +3812,461 @@
       </border>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog60.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="190" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="191" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="192" sheetId="1" source="E10" destination="F10" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="193" sId="1" odxf="1" dxf="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:F11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog61.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="194" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rm rId="195" sheetId="1" source="C13:D13" destination="C14:D14" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D13:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D14">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rrc rId="196" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C13" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="197" sId="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="198" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="199" sId="1">
+    <oc r="D10">
+      <v>8</v>
+    </oc>
+    <nc r="D10">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="200" sId="1">
+    <oc r="D11">
+      <v>4</v>
+    </oc>
+    <nc r="D11">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="201" sId="1">
+    <oc r="E13" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </oc>
+    <nc r="E13"/>
+  </rcc>
+  <rcc rId="202" sId="1" odxf="1" dxf="1">
+    <nc r="D13">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="203" sId="1" odxf="1" dxf="1">
+    <nc r="D14">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="204" sId="1">
+    <oc r="F10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F10"/>
+  </rcc>
+  <rcc rId="205" sId="1">
+    <oc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F11"/>
+  </rcc>
+  <rcc rId="206" sId="1">
+    <oc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="207" sId="1">
+    <oc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen</t>
+      </is>
+    </oc>
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="208" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:E11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="0">
+    <dxf>
+      <alignment horizontal="left" vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="209" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher, Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="210" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog62.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="211" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </oc>
+    <nc r="G6">
+      <v>40</v>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -1985,12 +4451,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="4">
-  <userInfo guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" name="Microsoft Office-Anwender" id="-1182387524" dateTime="2017-04-22T12:05:17"/>
-  <userInfo guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" name="Benni" id="-940673984" dateTime="2017-04-22T12:11:06"/>
-  <userInfo guid="{6E32143D-2DAC-4DA1-9C06-7DECE03B8640}" name="Microsoft Office-Anwender" id="-1182379380" dateTime="2017-04-22T12:25:45"/>
-  <userInfo guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" name="Microsoft Office-Anwender" id="-1182371220" dateTime="2017-04-22T12:28:01"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2256,383 +4717,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15">
-        <v>2</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="20" t="s">
-        <v>27</v>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="19">
-        <v>50</v>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="31">
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="8">
-        <v>8</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="13"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="18">
+        <v>4</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8">
-        <v>8</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="3"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="28">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="29">
+        <v>2</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="30">
+        <v>4</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="28">
+        <v>3</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="43">
+        <v>4</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="28">
+        <v>3</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="28">
+        <v>3</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="28">
+        <v>4</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="28">
+        <v>10</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="40">
+        <v>3</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="28">
         <v>6</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="8">
-        <v>4</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8">
-        <v>3</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="8">
-        <v>8</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="17">
-        <v>4</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="15">
-        <v>5</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="24"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="28">
+        <v>3</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="8">
-        <v>6</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="3"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="28">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="8">
-        <v>5</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="28">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8">
-        <v>4</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D24" s="8">
-        <v>2</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="8">
-        <v>2</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D26" s="8">
-        <v>10</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D27" s="8">
-        <v>10</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" s="8">
+        <v>5</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="28">
         <v>4</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="3"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="28">
+        <v>3</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="6"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="28">
+        <v>3</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="3"/>
     </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="28">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="3"/>
     </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
     </row>
-    <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="8">
+        <v>4</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="3"/>
     </row>
-    <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="8">
+        <v>2</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="3"/>
     </row>
-    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="8">
+        <v>2</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="3"/>
     </row>
-    <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="8">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="8">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G11" sqref="G11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+    </customSheetView>
+    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
+      <selection activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
     <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added hopefully final version of product backlog for first sprint
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="1135" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
     <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
-    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
-    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Storypoints pro Sprint:</t>
   </si>
   <si>
-    <t>Calvin</t>
-  </si>
-  <si>
     <t>1. Sprint bis hierher</t>
   </si>
   <si>
@@ -144,40 +141,13 @@
     <t>Reservierungen/Verkäufe anzeigen</t>
   </si>
   <si>
-    <t>Customer selection nach Saalplan</t>
-  </si>
-  <si>
     <t>Saalplan Sitzplätze</t>
   </si>
   <si>
     <t>Saalplan Sektoren</t>
   </si>
   <si>
-    <t>vllt noch in erstem Sprint?</t>
-  </si>
-  <si>
     <t>Martin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Martin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/Calvin</t>
-    </r>
   </si>
   <si>
     <t>Ticketverkauf, clientseitig</t>
@@ -192,14 +162,21 @@
     <t>Ticketreservierungen, serverseitig</t>
   </si>
   <si>
-    <t>Christopher, Calvin</t>
+    <t>Calvin/Martin</t>
+  </si>
+  <si>
+    <t>Martin/Calvin</t>
+  </si>
+  <si>
+    <t>Detailansicht von Reservierungen/
+Verkäufe inkl. Customer Selection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,13 +215,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -451,7 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,12 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -497,8 +460,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,7 +493,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{50242816-3825-4FDE-8AC5-9767A747207A}" diskRevisions="1" revisionId="211" version="19">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" diskRevisions="1" revisionId="226" version="24">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -850,6 +825,31 @@
     </sheetIdMap>
   </header>
   <header guid="{50242816-3825-4FDE-8AC5-9767A747207A}" dateTime="2017-05-07T17:26:12" maxSheetId="2" userName="Microsoft" r:id="rId67" minRId="211">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C45E9881-E23C-4AA3-AD22-D0D6759584D2}" dateTime="2017-05-07T23:22:25" maxSheetId="2" userName="Microsoft" r:id="rId68" minRId="212" maxRId="217">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F3D5534B-BCEC-4564-9E4B-CBF7F64C8926}" dateTime="2017-05-07T23:22:32" maxSheetId="2" userName="Microsoft" r:id="rId69" minRId="218">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F02534F4-8637-44B1-9333-E70767EDF8CC}" dateTime="2017-05-08T11:14:36" maxSheetId="2" userName="Microsoft" r:id="rId70" minRId="219" maxRId="223">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F1D55F0F-D3EF-4D54-9EE8-4F8AA68F9F44}" dateTime="2017-05-08T11:14:43" maxSheetId="2" userName="Microsoft" r:id="rId71" minRId="224" maxRId="226">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" dateTime="2017-05-08T11:15:27" maxSheetId="2" userName="Microsoft" r:id="rId72">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -4267,6 +4267,314 @@
       <v>40</v>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog63.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="212" sId="1" ref="A10:XFD10" action="insertRow"/>
+  <rcc rId="213" sId="1">
+    <oc r="D11">
+      <v>4</v>
+    </oc>
+    <nc r="D11">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="214" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/Verkäufe</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="215" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="216" sId="1">
+    <oc r="E5" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>Calvin/Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="217" sId="1">
+    <oc r="E6" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>Calvin/Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog64.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="218" sId="1">
+    <nc r="D10">
+      <v>2</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog65.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="219" sId="1">
+    <oc r="D10">
+      <v>2</v>
+    </oc>
+    <nc r="D10">
+      <v>5</v>
+    </nc>
+  </rcc>
+  <rrc rId="220" sId="1" ref="A9:XFD9" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A9:XFD9" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="A9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C9" t="inlineStr">
+        <is>
+          <t>Customer selection nach Saalplan</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0"/>
+          </patternFill>
+        </fill>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="D9">
+        <v>2</v>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="E9" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <sz val="11"/>
+              <rFont val="Calibri"/>
+              <family val="2"/>
+            </rPr>
+            <t>Martin</t>
+          </r>
+          <r>
+            <rPr>
+              <sz val="11"/>
+              <rFont val="Calibri"/>
+              <family val="2"/>
+            </rPr>
+            <t>/Calvin</t>
+          </r>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="F9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="H9" start="0" length="0">
+      <dxf/>
+    </rfmt>
+    <rfmt sheetId="1" sqref="I9" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rrc>
+  <rcc rId="221" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="222" sId="1">
+    <oc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher, Calvin</t>
+      </is>
+    </oc>
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="223" sId="1" odxf="1" dxf="1">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/Verkäufe</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/
+Verkäufe inkl. Customer Selection</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog66.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="224" sId="1">
+    <oc r="E17" t="inlineStr">
+      <is>
+        <t>vllt noch in erstem Sprint?</t>
+      </is>
+    </oc>
+    <nc r="E17"/>
+  </rcc>
+  <rcc rId="225" sId="1">
+    <oc r="E18" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E18"/>
+  </rcc>
+  <rcc rId="226" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </oc>
+    <nc r="E19"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog67.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E9">
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
 </revisions>
 </file>
 
@@ -4720,15 +5028,16 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4736,10 +5045,10 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="45"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
@@ -4754,7 +5063,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -4767,8 +5076,8 @@
       <c r="D5" s="17">
         <v>4</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>25</v>
+      <c r="E5" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="14" t="s">
@@ -4783,11 +5092,11 @@
       <c r="D6" s="18">
         <v>3</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>25</v>
+      <c r="E6" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <v>40</v>
       </c>
     </row>
@@ -4795,13 +5104,13 @@
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
       <c r="C7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="18">
         <v>4</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>35</v>
+      <c r="E7" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -4809,30 +5118,30 @@
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="28">
+        <v>37</v>
+      </c>
+      <c r="D8" s="27">
         <v>14</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="29">
-        <v>2</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>42</v>
+      <c r="C9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="28">
+        <v>5</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>44</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -4843,15 +5152,15 @@
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="30">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D10" s="29">
+        <v>3</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="F10" s="42"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -4860,32 +5169,32 @@
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="28">
+        <v>42</v>
+      </c>
+      <c r="D11" s="27">
         <v>3</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="F11" s="42"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="43">
+      <c r="C12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="40">
         <v>4</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>41</v>
+      <c r="E12" s="41" t="s">
+        <v>38</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
@@ -4895,12 +5204,12 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="25"/>
       <c r="C13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="28">
+        <v>39</v>
+      </c>
+      <c r="D13" s="27">
         <v>3</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -4909,12 +5218,12 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="28">
+        <v>40</v>
+      </c>
+      <c r="D14" s="27">
         <v>3</v>
       </c>
-      <c r="E14" s="36"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="19"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4925,10 +5234,10 @@
       <c r="C15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="27">
         <v>4</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="19"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -4936,9 +5245,9 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="28">
+        <v>36</v>
+      </c>
+      <c r="D16" s="27">
         <v>10</v>
       </c>
       <c r="G16" s="20"/>
@@ -4948,15 +5257,13 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="40">
+      <c r="C17" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="37">
         <v>3</v>
       </c>
-      <c r="E17" s="41" t="s">
-        <v>40</v>
-      </c>
+      <c r="E17" s="38"/>
       <c r="F17" s="19"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
@@ -4966,12 +5273,10 @@
       <c r="C18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <v>6</v>
       </c>
-      <c r="E18" s="37" t="s">
-        <v>25</v>
-      </c>
+      <c r="E18" s="34"/>
       <c r="F18" s="24"/>
       <c r="G18" s="3"/>
     </row>
@@ -4979,12 +5284,10 @@
       <c r="C19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <v>3</v>
       </c>
-      <c r="E19" s="38" t="s">
-        <v>28</v>
-      </c>
+      <c r="E19" s="35"/>
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
@@ -4992,7 +5295,7 @@
       <c r="C20" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="27">
         <v>8</v>
       </c>
       <c r="E20" s="11"/>
@@ -5002,7 +5305,7 @@
       <c r="C21" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="27">
         <v>4</v>
       </c>
       <c r="E21" s="15"/>
@@ -5087,10 +5390,10 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C29" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="28">
+      <c r="C29" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="27">
         <v>4</v>
       </c>
       <c r="E29" s="11"/>
@@ -5099,9 +5402,9 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="28">
+        <v>29</v>
+      </c>
+      <c r="D30" s="27">
         <v>3</v>
       </c>
       <c r="E30" s="11"/>
@@ -5110,9 +5413,9 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="28">
+        <v>28</v>
+      </c>
+      <c r="D31" s="27">
         <v>3</v>
       </c>
       <c r="E31" s="11"/>
@@ -5121,9 +5424,9 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="28">
+        <v>30</v>
+      </c>
+      <c r="D32" s="27">
         <v>1</v>
       </c>
       <c r="E32" s="11"/>
@@ -5232,23 +5535,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G11" sqref="G11"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
+      <selection activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
       <selection activeCell="G7" sqref="G7"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
-      <selection activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
+      <selection activeCell="G16" sqref="G16"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>

</xml_diff>

<commit_message>
Product Backlog new version
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
+    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
     <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -61,15 +63,6 @@
   </si>
   <si>
     <t>Veranstaltungsarten</t>
-  </si>
-  <si>
-    <t>Saalplan</t>
-  </si>
-  <si>
-    <t>Ticketverkauf</t>
-  </si>
-  <si>
-    <t>Ticketreservierungen</t>
   </si>
   <si>
     <t>Stornierung von Ticketreservierungen</t>
@@ -114,19 +107,7 @@
     <t>Storypoints pro Sprint:</t>
   </si>
   <si>
-    <t>Calvin</t>
-  </si>
-  <si>
-    <t>Benni</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>1. Sprint bis hierher</t>
-  </si>
-  <si>
-    <t>Martin</t>
   </si>
   <si>
     <t>Verantwortlicher:</t>
@@ -134,12 +115,68 @@
   <si>
     <t>Christopher</t>
   </si>
+  <si>
+    <t>einzelne News anzeigen</t>
+  </si>
+  <si>
+    <t>News erstellen</t>
+  </si>
+  <si>
+    <t>gesehene News anzeigen/ausblenden</t>
+  </si>
+  <si>
+    <t>Veranstaltungen/Performances anzeigen</t>
+  </si>
+  <si>
+    <t>Verkauf von ausgewählten Ticktes</t>
+  </si>
+  <si>
+    <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+  </si>
+  <si>
+    <t>Alex / Benni</t>
+  </si>
+  <si>
+    <t>Reservierungen/Verkäufe anzeigen</t>
+  </si>
+  <si>
+    <t>Saalplan Sitzplätze</t>
+  </si>
+  <si>
+    <t>Saalplan Sektoren</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Ticketverkauf, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, clientseitig</t>
+  </si>
+  <si>
+    <t>Ticketverkauf, serverseitig</t>
+  </si>
+  <si>
+    <t>Ticketreservierungen, serverseitig</t>
+  </si>
+  <si>
+    <t>Calvin/Martin</t>
+  </si>
+  <si>
+    <t>Martin/Calvin</t>
+  </si>
+  <si>
+    <t>Detailansicht von Reservierungen/
+Verkäufe inkl. Customer Selection</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +199,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -262,6 +332,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -276,33 +359,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -324,12 +385,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -337,21 +392,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -371,7 +493,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D940A152-4973-4D75-9614-BF1E9168855C}" diskRevisions="1" revisionId="98" version="32">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" diskRevisions="1" revisionId="226" version="24">
   <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -532,11 +654,214 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{66393CF5-0FDE-4512-8890-578A78AAC3E7}" dateTime="2017-04-29T13:17:41" maxSheetId="2" userName="Microsoft" r:id="rId33" minRId="99" maxRId="104">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{81D78350-56F2-4F79-8F34-9FA0C6006D6B}" dateTime="2017-04-29T13:17:53" maxSheetId="2" userName="Microsoft" r:id="rId34">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5BCC245A-D038-4ED2-846F-3E88B59B5762}" dateTime="2017-04-29T13:19:00" maxSheetId="2" userName="Microsoft" r:id="rId35" minRId="105" maxRId="110">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{101AB0F5-6614-467B-8A51-2AE4FF720756}" dateTime="2017-04-29T13:19:09" maxSheetId="2" userName="Microsoft" r:id="rId36" minRId="111">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C83FF58A-9A07-4F9A-9AC7-66EA08B9EB04}" dateTime="2017-04-29T17:39:28" maxSheetId="2" userName="Microsoft" r:id="rId37" minRId="112" maxRId="113">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B023F33C-AA89-488A-BBF9-02922DB5D2FA}" dateTime="2017-04-29T17:40:36" maxSheetId="2" userName="Microsoft" r:id="rId38" minRId="114" maxRId="119">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{75D88859-5FC7-4B07-8D78-F6D07ED55CFD}" dateTime="2017-04-29T17:41:43" maxSheetId="2" userName="Microsoft" r:id="rId39" minRId="120" maxRId="128">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{36D6F9EE-A4EF-4402-ADFB-2D1AF6D063AB}" dateTime="2017-04-29T17:42:05" maxSheetId="2" userName="Microsoft" r:id="rId40" minRId="129">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B16787EC-4036-4C68-A548-F79083FC9DCF}" dateTime="2017-04-29T17:44:27" maxSheetId="2" userName="Microsoft" r:id="rId41" minRId="130" maxRId="134">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5D044380-438D-45CC-BBA3-EB80158F26AA}" dateTime="2017-04-29T17:45:11" maxSheetId="2" userName="Microsoft" r:id="rId42" minRId="135" maxRId="138">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5C76CD5F-F0CF-4BA9-BB8B-425EAAE868E1}" dateTime="2017-04-29T17:45:58" maxSheetId="2" userName="Microsoft" r:id="rId43" minRId="139">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5F0E435C-195A-4E12-ABF6-24B398812027}" dateTime="2017-04-29T17:46:18" maxSheetId="2" userName="Microsoft" r:id="rId44" minRId="140">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{18EF123C-08DB-4690-B5AC-401D3A2BED42}" dateTime="2017-04-29T17:49:44" maxSheetId="2" userName="Microsoft" r:id="rId45" minRId="141">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{09C0619A-3ABD-48AF-81FF-EDEC2AC796BC}" dateTime="2017-04-29T17:50:18" maxSheetId="2" userName="Microsoft" r:id="rId46" minRId="142">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{603823E5-CE07-4017-8D88-4645AD050333}" dateTime="2017-04-29T17:51:09" maxSheetId="2" userName="Microsoft" r:id="rId47" minRId="143" maxRId="145">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{01E1650E-2E16-4B9F-AC6F-690256DD718A}" dateTime="2017-04-30T14:48:59" maxSheetId="2" userName="Alex" r:id="rId48" minRId="146" maxRId="165">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{16014D3B-0EFA-4026-924D-8B091FF9FA05}" dateTime="2017-04-30T14:49:20" maxSheetId="2" userName="Alex" r:id="rId49">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CE36F0C9-B20E-47E7-8744-736AED355D2C}" dateTime="2017-04-30T14:49:46" maxSheetId="2" userName="Alex" r:id="rId50">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CC968181-75FD-4583-8D56-6CCAB2E56C0D}" dateTime="2017-04-30T14:51:39" maxSheetId="2" userName="Alex" r:id="rId51" minRId="166">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A587955F-CBDA-4235-945C-32CE722EBAE5}" dateTime="2017-04-30T14:51:40" maxSheetId="2" userName="Alex" r:id="rId52">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FD6FC766-CC2B-4CF6-8884-ED02F511E3A7}" dateTime="2017-05-01T18:48:28" maxSheetId="2" userName="Microsoft" r:id="rId53">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6BBE8D34-9650-4684-A45F-BA49B93F22F5}" dateTime="2017-05-01T18:48:47" maxSheetId="2" userName="Microsoft" r:id="rId54" minRId="167">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A133C022-AFE6-447E-BECA-8B93C5221737}" dateTime="2017-05-03T16:06:28" maxSheetId="2" userName="Martin Klampfer" r:id="rId55" minRId="168" maxRId="176">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{889BB63A-29AE-4B6E-85A4-F158D5946810}" dateTime="2017-05-03T16:06:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId56" minRId="177" maxRId="178">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{19038F75-9BEF-4375-9595-4ED078EB4966}" dateTime="2017-05-03T16:08:34" maxSheetId="2" userName="Martin Klampfer" r:id="rId57" minRId="179" maxRId="184">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6AF878D6-9310-4021-BBDE-8E4786BC598C}" dateTime="2017-05-03T16:08:54" maxSheetId="2" userName="Martin Klampfer" r:id="rId58">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{566CAB0B-B727-4D41-8831-C2010EC0A46F}" dateTime="2017-05-03T16:09:49" maxSheetId="2" userName="Martin Klampfer" r:id="rId59" minRId="185">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9A2E6002-35E9-4C02-A72A-3D5A8BF0E06C}" dateTime="2017-05-03T16:09:56" maxSheetId="2" userName="Martin Klampfer" r:id="rId60">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7C64980B-A064-4084-8801-1814945BDF5E}" dateTime="2017-05-03T16:10:00" maxSheetId="2" userName="Martin Klampfer" r:id="rId61">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{874C0D29-8150-4D0C-9A0D-8ED1CF64EE82}" dateTime="2017-05-07T17:09:01" maxSheetId="2" userName="Microsoft" r:id="rId62" minRId="186" maxRId="188">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3F184119-29BE-43A1-AEDE-BB639519E443}" dateTime="2017-05-07T17:09:09" maxSheetId="2" userName="Microsoft" r:id="rId63" minRId="189">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6591666E-586B-444E-9942-3D0D6E6B6951}" dateTime="2017-05-07T17:09:19" maxSheetId="2" userName="Microsoft" r:id="rId64">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2C4B1529-DFDB-46F2-B2FF-B354077682B9}" dateTime="2017-05-07T17:13:28" maxSheetId="2" userName="Microsoft" r:id="rId65" minRId="190" maxRId="193">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1292FC90-6409-4788-AE41-4BD648128DC5}" dateTime="2017-05-07T17:14:59" maxSheetId="2" userName="Microsoft" r:id="rId66" minRId="194" maxRId="210">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{50242816-3825-4FDE-8AC5-9767A747207A}" dateTime="2017-05-07T17:26:12" maxSheetId="2" userName="Microsoft" r:id="rId67" minRId="211">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C45E9881-E23C-4AA3-AD22-D0D6759584D2}" dateTime="2017-05-07T23:22:25" maxSheetId="2" userName="Microsoft" r:id="rId68" minRId="212" maxRId="217">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F3D5534B-BCEC-4564-9E4B-CBF7F64C8926}" dateTime="2017-05-07T23:22:32" maxSheetId="2" userName="Microsoft" r:id="rId69" minRId="218">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F02534F4-8637-44B1-9333-E70767EDF8CC}" dateTime="2017-05-08T11:14:36" maxSheetId="2" userName="Microsoft" r:id="rId70" minRId="219" maxRId="223">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F1D55F0F-D3EF-4D54-9EE8-4F8AA68F9F44}" dateTime="2017-05-08T11:14:43" maxSheetId="2" userName="Microsoft" r:id="rId71" minRId="224" maxRId="226">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" dateTime="2017-05-08T11:15:27" maxSheetId="2" userName="Microsoft" r:id="rId72">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -565,6 +890,333 @@
 </file>
 
 <file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog110.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="146" sId="1">
+    <oc r="C7" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Veramstaöti</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="147" sheetId="1" source="C8" destination="C7" sourceSheetId="1">
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>Veramstaöti</t>
+        </is>
+      </nc>
+      <ndxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+  </rm>
+  <rm rId="148" sheetId="1" source="B8" destination="C8" sourceSheetId="1"/>
+  <rm rId="149" sheetId="1" source="D8" destination="F7" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F7" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="150" sheetId="1" source="D7" destination="D8" sourceSheetId="1"/>
+  <rm rId="151" sheetId="1" source="F7" destination="D7" sourceSheetId="1"/>
+  <rcc rId="152" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="153" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Alex</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C8" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C8">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="154" sheetId="1" source="C8" destination="I9" sourceSheetId="1"/>
+  <rcc rId="155" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8"/>
+  </rcc>
+  <rm rId="156" sheetId="1" source="C9:G10" destination="C8:G9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="D8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F8" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G8" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="157" sId="1">
+    <nc r="D10">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rcc rId="158" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10 D10 C10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="159" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </oc>
+    <nc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C9:G9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C9 D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rm rId="160" sheetId="1" source="C11:D11" destination="G12:H12" sourceSheetId="1"/>
+  <rm rId="161" sheetId="1" source="C12:E12" destination="C11:E11" sourceSheetId="1"/>
+  <rm rId="162" sheetId="1" source="G12:H12" destination="C12:D12" sourceSheetId="1"/>
+  <rrc rId="163" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rcc rId="164" sId="1">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Reservierungen/Verkäufe anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="165" sId="1">
+    <nc r="D12">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog1111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="53" sId="1">
     <nc r="D16">
@@ -595,6 +1247,25 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog112.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="166" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="1">
@@ -619,6 +1290,13 @@
 </file>
 
 <file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
+  <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog141.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="60" sId="1">
     <nc r="D7">
@@ -1422,6 +2100,480 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="99" sId="1">
+    <oc r="D8">
+      <v>8</v>
+    </oc>
+    <nc r="D8">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rrc rId="100" sId="1" ref="A8:XFD8" action="insertRow"/>
+  <rcc rId="101" sId="1">
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1">
+    <nc r="D8">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="1">
+    <oc r="D5">
+      <v>2</v>
+    </oc>
+    <nc r="D5">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="1">
+    <oc r="D6">
+      <v>2</v>
+    </oc>
+    <nc r="D6">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D5:D6 C8:D8" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D9" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="105" sheetId="1" source="C10:E10" destination="C34:E34" sourceSheetId="1"/>
+  <rrc rId="106" sId="1" ref="A10:XFD10" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A10:XFD10" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G10" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="107" sId="1" ref="A12:XFD12" action="insertRow"/>
+  <rm rId="108" sheetId="1" source="C34:E34" destination="C12:E12" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C12" start="0" length="0">
+      <dxf>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E12" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="109" sheetId="1" source="A15:B15" destination="A11:B11" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="C11:E11" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:D15">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D15">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A11:B11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="110" sId="1">
+    <oc r="G6">
+      <v>50</v>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="111" sId="1">
+    <oc r="D9">
+      <v>20</v>
+    </oc>
+    <nc r="D9">
+      <v>24</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="112" sId="1">
+    <oc r="D8">
+      <v>2</v>
+    </oc>
+    <nc r="D8">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="113" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 45</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="114" sId="1">
+    <oc r="D9">
+      <v>24</v>
+    </oc>
+    <nc r="D9">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="1">
+    <oc r="E14" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E14"/>
+  </rcc>
+  <rcc rId="116" sId="1">
+    <oc r="E15" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E15"/>
+  </rcc>
+  <rrc rId="117" sId="1" ref="A23:XFD23" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D23" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="118" sId="1">
+    <nc r="C23" t="inlineStr">
+      <is>
+        <t>einzelne News anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="1">
+    <nc r="D23">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C23:D23" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="120" sId="1" ref="A24:XFD24" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C24" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="121" sId="1" odxf="1" dxf="1">
+    <nc r="D24">
+      <v>3</v>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="122" sId="1">
+    <nc r="C24" t="inlineStr">
+      <is>
+        <t>News erstellen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="123" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D25" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="124" sId="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>gesehene News anzeigen/ausblenden</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="125" sheetId="1" source="C24:D24" destination="C35:D35" sourceSheetId="1"/>
+  <rm rId="126" sheetId="1" source="C23:D23" destination="C24:D24" sourceSheetId="1"/>
+  <rm rId="127" sheetId="1" source="C35:D35" destination="C23:D23" sourceSheetId="1"/>
+  <rcc rId="128" sId="1">
+    <nc r="D25">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rm rId="11" sheetId="1" source="C18" destination="C24" sourceSheetId="1">
@@ -1448,6 +2600,413 @@
   <rm rId="13" sheetId="1" source="C24" destination="C16" sourceSheetId="1"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
   <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="129" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 51</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C5:D6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog41.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="130" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen anzeigen</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Veranstaltungen/Performances anzeigen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="131" sId="1" ref="A9:XFD9" action="insertRow"/>
+  <rm rId="132" sheetId="1" source="C10:E10" destination="C9:E9" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E9" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcc rId="133" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Verkauf von ausgewählten Ticktes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D10" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:D10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="134" sId="1">
+    <nc r="D10">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D10">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog42.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="135" sId="1" ref="A10:XFD10" action="insertRow"/>
+  <rcc rId="136" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="137" sId="1">
+    <nc r="D10">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog43.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C10:G10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C10:G10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="139" sId="1" odxf="1" dxf="1">
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog44.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="140" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 52</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog45.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="141" sId="1">
+    <oc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E10"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog46.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="142" sId="1">
+    <oc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????</t>
+      </is>
+    </oc>
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>soll das überhaupt im selben
+Fenster wie Saalplan sein????
+eher zuerst Kunde auswählen,
+danach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="143" sId="1" ref="A25:XFD25" action="insertRow"/>
+  <rcc rId="144" sId="1" odxf="1" dxf="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+      </is>
+    </nc>
+    <odxf>
+      <alignment vertical="bottom" wrapText="0" readingOrder="0"/>
+    </odxf>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="145" sId="1">
+    <nc r="D25">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C25:D25" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog48.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E8:E13" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I8:I13" start="0" length="0">
+    <dxf>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D7:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:E14" start="0" length="0">
+    <dxf>
+      <border>
+        <left/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E14:H14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E8:I15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D8:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog49.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="167" sId="1">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -1726,6 +3285,458 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog50.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="168" sId="1">
+    <oc r="G9" t="inlineStr">
+      <is>
+        <t>Platzierung: später überlegen</t>
+      </is>
+    </oc>
+    <nc r="G9"/>
+  </rcc>
+  <rm rId="169" sheetId="1" source="A14:B14" destination="A12:B12" sourceSheetId="1"/>
+  <rcc rId="170" sId="1">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection in Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Customer selection nach Saalplan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="A7:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C7:D18" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="171" sId="1">
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="172" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="173" sheetId="1" source="C13:D13" destination="C39:D39" sourceSheetId="1"/>
+  <rm rId="174" sheetId="1" source="C14:E14" destination="C13:E13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E13" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rm rId="175" sheetId="1" source="C39:D39" destination="C14:D14" sourceSheetId="1"/>
+  <rm rId="176" sheetId="1" source="A12" destination="A13" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="A13" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="177" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="178" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 56</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog52.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="179" sheetId="1" source="A14:F37" destination="A15:F38" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="E38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F38" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="180" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Saalplan Sitzplätze</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="181" sId="1">
+    <nc r="D14">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="182" sId="1">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Saalplan Sektoren</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="183" sId="1">
+    <oc r="D8">
+      <v>20</v>
+    </oc>
+    <nc r="D8">
+      <v>14</v>
+    </nc>
+  </rcc>
+  <rcc rId="184" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 53</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="delete"/>
+  <rcv guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog53.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C27:D30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog54.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcc rId="185" sId="1">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>vllt noch in erstem Sprint?</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog55.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D14:D17" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog56.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D10:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog57.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="186" sId="1">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>(Alex / Benni) Calvin?</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="187" sId="1">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Martin/Christopher</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14:D14">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="188" sheetId="1" source="A13" destination="A12" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="E13" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15:E17" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:F15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog58.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="189" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 47</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog59.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E5:E7" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:E12" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rfmt sheetId="1" sqref="C22" start="0" length="0">
@@ -1799,6 +3810,769 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog60.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="190" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="191" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="192" sheetId="1" source="E10" destination="F10" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="F10" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rm>
+  <rcc rId="193" sId="1" odxf="1" dxf="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:F11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog61.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="194" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rm rId="195" sheetId="1" source="C13:D13" destination="C14:D14" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D14" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+        </border>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="0">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D13" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D13:D14" start="0" length="0">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:D14">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C12:D12" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rrc rId="196" sId="1" ref="A14:XFD14" action="insertRow"/>
+  <rfmt sheetId="1" sqref="C13" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C14" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:C14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="197" sId="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="198" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, clientseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="199" sId="1">
+    <oc r="D10">
+      <v>8</v>
+    </oc>
+    <nc r="D10">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="200" sId="1">
+    <oc r="D11">
+      <v>4</v>
+    </oc>
+    <nc r="D11">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="201" sId="1">
+    <oc r="E13" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </oc>
+    <nc r="E13"/>
+  </rcc>
+  <rcc rId="202" sId="1" odxf="1" dxf="1">
+    <nc r="D13">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="203" sId="1" odxf="1" dxf="1">
+    <nc r="D14">
+      <v>3</v>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="204" sId="1">
+    <oc r="F10" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F10"/>
+  </rcc>
+  <rcc rId="205" sId="1">
+    <oc r="F11" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> - vllt mal nur Serverseitig, wäre ganz wichtig einmal</t>
+      </is>
+    </oc>
+    <nc r="F11"/>
+  </rcc>
+  <rcc rId="206" sId="1">
+    <oc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf</t>
+      </is>
+    </oc>
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Ticketverkauf, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="207" sId="1">
+    <oc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen</t>
+      </is>
+    </oc>
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>Ticketreservierungen, serverseitig</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="208" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 43</t>
+      </is>
+    </oc>
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C10:E11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E10" start="0" length="0">
+    <dxf>
+      <alignment horizontal="left" vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="209" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher, Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="210" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin ?</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>/Calvin</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog62.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="211" sId="1">
+    <oc r="G6" t="inlineStr">
+      <is>
+        <t>wären: 38</t>
+      </is>
+    </oc>
+    <nc r="G6">
+      <v>40</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog63.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="212" sId="1" ref="A10:XFD10" action="insertRow"/>
+  <rcc rId="213" sId="1">
+    <oc r="D11">
+      <v>4</v>
+    </oc>
+    <nc r="D11">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="214" sId="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/Verkäufe</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="215" sId="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="216" sId="1">
+    <oc r="E5" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>Calvin/Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="217" sId="1">
+    <oc r="E6" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>Calvin/Martin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog64.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="218" sId="1">
+    <nc r="D10">
+      <v>2</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog65.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="219" sId="1">
+    <oc r="D10">
+      <v>2</v>
+    </oc>
+    <nc r="D10">
+      <v>5</v>
+    </nc>
+  </rcc>
+  <rrc rId="220" sId="1" ref="A9:XFD9" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A9:XFD9" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="A9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C9" t="inlineStr">
+        <is>
+          <t>Customer selection nach Saalplan</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0"/>
+          </patternFill>
+        </fill>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="D9">
+        <v>2</v>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="E9" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <b/>
+              <sz val="11"/>
+              <rFont val="Calibri"/>
+              <family val="2"/>
+            </rPr>
+            <t>Martin</t>
+          </r>
+          <r>
+            <rPr>
+              <sz val="11"/>
+              <rFont val="Calibri"/>
+              <family val="2"/>
+            </rPr>
+            <t>/Calvin</t>
+          </r>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="F9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G9" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="H9" start="0" length="0">
+      <dxf/>
+    </rfmt>
+    <rfmt sheetId="1" sqref="I9" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rrc>
+  <rcc rId="221" sId="1">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Martin</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Martin/Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="222" sId="1">
+    <oc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher, Calvin</t>
+      </is>
+    </oc>
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="223" sId="1" odxf="1" dxf="1">
+    <oc r="C9" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/Verkäufe</t>
+      </is>
+    </oc>
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>Detailansicht von Reservierungen/
+Verkäufe inkl. Customer Selection</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog66.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="224" sId="1">
+    <oc r="E17" t="inlineStr">
+      <is>
+        <t>vllt noch in erstem Sprint?</t>
+      </is>
+    </oc>
+    <nc r="E17"/>
+  </rcc>
+  <rcc rId="225" sId="1">
+    <oc r="E18" t="inlineStr">
+      <is>
+        <t>Calvin</t>
+      </is>
+    </oc>
+    <nc r="E18"/>
+  </rcc>
+  <rcc rId="226" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <t>Christopher</t>
+      </is>
+    </oc>
+    <nc r="E19"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog67.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E9">
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
     </dxf>
   </rfmt>
 </revisions>
@@ -1985,12 +4759,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="4">
-  <userInfo guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" name="Microsoft Office-Anwender" id="-1182387524" dateTime="2017-04-22T12:05:17"/>
-  <userInfo guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" name="Benni" id="-940673984" dateTime="2017-04-22T12:11:06"/>
-  <userInfo guid="{6E32143D-2DAC-4DA1-9C06-7DECE03B8640}" name="Microsoft Office-Anwender" id="-1182379380" dateTime="2017-04-22T12:25:45"/>
-  <userInfo guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" name="Microsoft Office-Anwender" id="-1182371220" dateTime="2017-04-22T12:28:01"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2256,383 +5025,541 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="45"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15">
-        <v>2</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="20" t="s">
-        <v>27</v>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="19">
-        <v>50</v>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="30">
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="8">
-        <v>8</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="13"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="18">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8">
-        <v>8</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="3"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="27">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="28">
+        <v>5</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="29">
+        <v>3</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="27">
+        <v>3</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="40">
+        <v>4</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="27">
+        <v>3</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="27">
+        <v>3</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="27">
+        <v>4</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="27">
+        <v>10</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="37">
+        <v>3</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="27">
         <v>6</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="8">
-        <v>4</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8">
-        <v>3</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="8">
-        <v>8</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="17">
-        <v>4</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="15">
-        <v>5</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="27">
+        <v>3</v>
+      </c>
+      <c r="E19" s="35"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="8">
-        <v>6</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="3"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="27">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="8">
-        <v>5</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="27">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8">
-        <v>4</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D24" s="8">
-        <v>2</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="8">
-        <v>2</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D26" s="8">
-        <v>10</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D27" s="8">
-        <v>10</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" s="8">
+        <v>5</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="27">
         <v>4</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="3"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="27">
+        <v>3</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="6"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="27">
+        <v>3</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="3"/>
     </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="3"/>
     </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
     </row>
-    <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="8">
+        <v>4</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="3"/>
     </row>
-    <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="8">
+        <v>2</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="3"/>
     </row>
-    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="8">
+        <v>2</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="3"/>
     </row>
-    <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="8">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="8">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G14" sqref="G14"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{C5B156C7-D343-4698-A97F-B19105873C1E}">
+      <selection activeCell="G16" sqref="G16"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+    </customSheetView>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+    </customSheetView>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
+      <selection activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
deleted unnecessary files and updated mockup and product backlog - working on Designdocument right now
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="12270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
     <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
-    <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="971" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Punkte:</t>
   </si>
   <si>
-    <t>Mehrsprachigkeit - laufend</t>
-  </si>
-  <si>
     <t>Storypoints pro Sprint:</t>
   </si>
   <si>
@@ -129,10 +126,6 @@
   </si>
   <si>
     <t>Verkauf von ausgewählten Ticktes</t>
-  </si>
-  <si>
-    <t>Übersicht alles Rechnungen/Reservierungen
-Stornierungen und PDF neu drucken</t>
   </si>
   <si>
     <t>Alex / Benni</t>
@@ -170,6 +163,34 @@
   <si>
     <t>Detailansicht von Reservierungen/
 Verkäufe inkl. Customer Selection</t>
+  </si>
+  <si>
+    <t>2. Sprint bis hierher</t>
+  </si>
+  <si>
+    <t>Martin / Calvin</t>
+  </si>
+  <si>
+    <t>Calvin/Christopfer</t>
+  </si>
+  <si>
+    <t>3. Sprint bis hierher</t>
+  </si>
+  <si>
+    <t>Christopher?</t>
+  </si>
+  <si>
+    <t>Alex/Benni ?</t>
+  </si>
+  <si>
+    <t>Calvin/Martin?</t>
+  </si>
+  <si>
+    <t>ist doch bereits erledigt oder?</t>
+  </si>
+  <si>
+    <t>Übersicht aller Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
   </si>
 </sst>
 </file>
@@ -241,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -359,11 +380,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -387,10 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,35 +452,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,17 +468,48 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,167 +529,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" diskRevisions="1" revisionId="226" version="24">
-  <header guid="{343B322A-93CA-4A38-ABF9-DA493A34E67D}" dateTime="2017-04-22T12:00:25" maxSheetId="2" userName="Microsoft" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8AA03EB2-5198-4FD0-B3DB-6365D7F5298C}" dateTime="2017-04-22T12:00:58" maxSheetId="2" userName="Microsoft" r:id="rId2" minRId="1" maxRId="3">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9A2BAA34-DCC6-41A4-9D6C-7A56A92F07C0}" dateTime="2017-04-22T12:04:59" maxSheetId="2" userName="Microsoft" r:id="rId3" minRId="4" maxRId="10">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C659DEFB-A3D2-4D76-82FE-0B5D4F3B1794}" dateTime="2017-04-22T12:05:11" maxSheetId="2" userName="Microsoft" r:id="rId4" minRId="11" maxRId="13">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A26451FE-13C2-4B57-B9C0-43333E8C1C24}" dateTime="2017-04-22T12:07:55" maxSheetId="2" userName="Microsoft" r:id="rId5" minRId="14" maxRId="32">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A1BE463F-6F48-4C19-8C14-473CD227E63D}" dateTime="2017-04-22T12:08:07" maxSheetId="2" userName="Microsoft" r:id="rId6">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F3925465-1EBE-42E9-B55C-D8EA468F51D3}" dateTime="2017-04-22T12:09:57" maxSheetId="2" userName="Microsoft" r:id="rId7" minRId="33" maxRId="39">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{328C0DDA-A665-4E16-AFC2-5E14E32A3B78}" dateTime="2017-04-22T12:10:18" maxSheetId="2" userName="Microsoft" r:id="rId8" minRId="40" maxRId="41">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{2BCC01BF-3126-4E7F-A421-83C1085D8A95}" dateTime="2017-04-22T12:12:03" maxSheetId="2" userName="Microsoft" r:id="rId9" minRId="42" maxRId="48">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{3ADA1521-C996-4975-8C46-35228A54E080}" dateTime="2017-04-22T12:16:17" maxSheetId="2" userName="Microsoft" r:id="rId10" minRId="49" maxRId="52">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{EA298982-26DD-4571-814F-51D4AE1CC0F0}" dateTime="2017-04-22T12:18:33" maxSheetId="2" userName="Benni" r:id="rId11" minRId="53" maxRId="57">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A41D54A9-9812-4D59-A3E7-F1ED17F6ECC3}" dateTime="2017-04-22T12:18:38" maxSheetId="2" userName="Benni" r:id="rId12" minRId="58">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8636A0AC-F284-4967-BF88-D89E995501BE}" dateTime="2017-04-22T12:19:01" maxSheetId="2" userName="Benni" r:id="rId13" minRId="59">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{888E1674-E1D7-48E7-8754-2BE846E233CC}" dateTime="2017-04-22T12:21:08" maxSheetId="2" userName="Benni" r:id="rId14" minRId="60" maxRId="61">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{7EC6220D-6C3E-4B07-9FB5-9CEC2ECDB029}" dateTime="2017-04-22T12:21:52" maxSheetId="2" userName="Benni" r:id="rId15" minRId="62" maxRId="63">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1606A72A-73BB-4611-AFC9-C958A86A38FD}" dateTime="2017-04-22T12:23:32" maxSheetId="2" userName="Benni" r:id="rId16" minRId="64">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1EA72236-60CD-4897-BCD5-FEC9933BB1A3}" dateTime="2017-04-22T12:24:14" maxSheetId="2" userName="Benni" r:id="rId17" minRId="65">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6E32143D-2DAC-4DA1-9C06-7DECE03B8640}" dateTime="2017-04-22T12:25:32" maxSheetId="2" userName="Benni" r:id="rId18" minRId="66" maxRId="67">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{AE88175A-5D46-400B-8572-297C36964A01}" dateTime="2017-04-22T12:26:58" maxSheetId="2" userName="Benni" r:id="rId19" minRId="68" maxRId="70">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1875917A-5559-445B-A658-6CA6F04976AD}" dateTime="2017-04-22T12:27:06" maxSheetId="2" userName="Benni" r:id="rId20" minRId="71">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{45B4032A-6310-402E-8D5E-61943BBCF2F9}" dateTime="2017-04-22T12:27:24" maxSheetId="2" userName="Benni" r:id="rId21" minRId="72">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E04E7876-87D7-428C-9E7C-8C3ECFC0FB71}" dateTime="2017-04-24T21:11:20" maxSheetId="2" userName="Microsoft" r:id="rId22" minRId="73" maxRId="80">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{23638F32-B4DA-40C3-9A47-E667A1F818C4}" dateTime="2017-04-24T21:11:45" maxSheetId="2" userName="Microsoft" r:id="rId23" minRId="81" maxRId="82">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DD8DD0D0-EFBD-4761-B0FA-1800ACB3F902}" dateTime="2017-04-24T21:13:56" maxSheetId="2" userName="Microsoft" r:id="rId24">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4869E5F4-950E-425A-9F85-C486B4CACBAB}" dateTime="2017-04-24T21:16:16" maxSheetId="2" userName="Microsoft" r:id="rId25" minRId="83">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FF4CC62A-F7DE-48EA-998C-54581DC04D97}" dateTime="2017-04-24T21:22:57" maxSheetId="2" userName="Microsoft" r:id="rId26" minRId="84" maxRId="89">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F0D33547-2A3F-4C5E-AFE9-E47388F393EB}" dateTime="2017-04-24T21:23:14" maxSheetId="2" userName="Microsoft" r:id="rId27">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F43B1A8A-AF05-4510-B16C-8814B8211959}" dateTime="2017-04-24T21:24:19" maxSheetId="2" userName="Microsoft" r:id="rId28" minRId="90" maxRId="93">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0ECB1E76-7103-460E-BE6F-38C41B57772F}" dateTime="2017-04-24T21:26:17" maxSheetId="2" userName="Microsoft" r:id="rId29" minRId="94" maxRId="97">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4A6F4A86-D4ED-4EA4-8B51-6A32563769E8}" dateTime="2017-04-24T21:26:29" maxSheetId="2" userName="Microsoft" r:id="rId30">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{76A35DCA-5D1E-4E72-A3F3-5FD70A23A358}" dateTime="2017-04-24T21:26:44" maxSheetId="2" userName="Microsoft" r:id="rId31" minRId="98">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D940A152-4973-4D75-9614-BF1E9168855C}" dateTime="2017-04-24T21:26:47" maxSheetId="2" userName="Microsoft" r:id="rId32">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AE1D7BD5-45E0-4B19-9F38-030FB29CC010}" diskRevisions="1" revisionId="278" version="38">
   <header guid="{66393CF5-0FDE-4512-8890-578A78AAC3E7}" dateTime="2017-04-29T13:17:41" maxSheetId="2" userName="Microsoft" r:id="rId33" minRId="99" maxRId="104">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -850,6 +726,76 @@
     </sheetIdMap>
   </header>
   <header guid="{DFE29802-CE7F-462C-8200-B5B178FA9E0D}" dateTime="2017-05-08T11:15:27" maxSheetId="2" userName="Microsoft" r:id="rId72">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B7332BE5-164E-4387-8C18-B3206B81A70E}" dateTime="2017-05-10T22:15:45" maxSheetId="2" userName="Microsoft" r:id="rId73" minRId="227" maxRId="229">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DE3D47BC-A4EB-410B-A9CD-BF5548C90EBA}" dateTime="2017-05-10T22:16:08" maxSheetId="2" userName="Microsoft" r:id="rId74" minRId="230">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{297A4F0A-F30C-4269-9E06-A827B7B5C7CE}" dateTime="2017-05-10T22:17:17" maxSheetId="2" userName="Microsoft" r:id="rId75" minRId="231" maxRId="234">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0E7EC024-C74D-4166-BD9C-B058335999C4}" dateTime="2017-05-10T22:18:15" maxSheetId="2" userName="Microsoft" r:id="rId76" minRId="235">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6D67104E-9692-4EB5-A708-D75F28C04361}" dateTime="2017-05-10T22:21:11" maxSheetId="2" userName="Microsoft" r:id="rId77" minRId="236" maxRId="246">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C5F8C6FF-6E43-41C9-B52D-BF8D0ED03466}" dateTime="2017-05-25T12:19:45" maxSheetId="2" userName="Microsoft" r:id="rId78" minRId="247" maxRId="257">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{91DD5137-3875-47CF-A842-C91EAD18DCCB}" dateTime="2017-05-25T12:21:01" maxSheetId="2" userName="Microsoft" r:id="rId79" minRId="258" maxRId="260">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{97559571-7948-479A-BCF0-DF37BE8B43BF}" dateTime="2017-05-25T12:21:21" maxSheetId="2" userName="Microsoft" r:id="rId80" minRId="261" maxRId="263">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C2AFA1C6-5944-41AF-8759-21D7A7FFB86D}" dateTime="2017-05-25T12:21:41" maxSheetId="2" userName="Microsoft" r:id="rId81" minRId="264" maxRId="271">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FDCBD257-ECB2-44E5-9122-83E4EC6BFF99}" dateTime="2017-05-25T12:23:07" maxSheetId="2" userName="Microsoft" r:id="rId82" minRId="272" maxRId="275">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B4A3D655-98B6-49E6-AAFB-B2FD8EB76D8C}" dateTime="2017-05-25T12:23:21" maxSheetId="2" userName="Microsoft" r:id="rId83" minRId="276" maxRId="277">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E588991D-66B7-4976-97EE-3B9D3CB41DE1}" dateTime="2017-05-25T12:23:29" maxSheetId="2" userName="Microsoft" r:id="rId84">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{26F0FA90-DE0E-488F-8F85-B59434695BB1}" dateTime="2017-05-25T12:23:41" maxSheetId="2" userName="Microsoft" r:id="rId85">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AE1D7BD5-45E0-4B19-9F38-030FB29CC010}" dateTime="2017-05-25T12:31:13" maxSheetId="2" userName="Microsoft" r:id="rId86" minRId="278">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -861,31 +807,6 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
   <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="49" sId="1">
-    <nc r="D23">
-      <v>4</v>
-    </nc>
-  </rcc>
-  <rcc rId="50" sId="1">
-    <nc r="D24">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="51" sId="1">
-    <nc r="D25">
-      <v>2</v>
-    </nc>
-  </rcc>
-  <rcc rId="52" sId="1">
-    <nc r="D21">
-      <v>5</v>
-    </nc>
-  </rcc>
 </revisions>
 </file>
 
@@ -1212,41 +1133,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog111.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog1111.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="53" sId="1">
-    <nc r="D16">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="54" sId="1">
-    <nc r="D17">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="55" sId="1">
-    <nc r="D18">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="56" sId="1">
-    <nc r="D19">
-      <v>1</v>
-    </nc>
-  </rcc>
-  <rcc rId="57" sId="1">
-    <nc r="D15">
-      <v>5</v>
-    </nc>
-  </rcc>
-  <rcv guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog112.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="166" sId="1">
@@ -1266,29 +1152,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="58" sId="1">
-    <nc r="D20">
-      <v>2</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="59" sId="1">
-    <oc r="D20">
-      <v>2</v>
-    </oc>
-    <nc r="D20">
-      <v>6</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcv guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" action="delete"/>
@@ -1296,807 +1159,16 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog141.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="60" sId="1">
-    <nc r="D7">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="61" sId="1">
-    <nc r="D8">
-      <v>8</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="62" sId="1">
-    <nc r="D9">
-      <v>6</v>
-    </nc>
-  </rcc>
-  <rcc rId="63" sId="1">
-    <nc r="D10">
-      <v>4</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="64" sId="1">
-    <nc r="D12">
-      <v>6</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="65" sId="1">
-    <oc r="D12">
-      <v>6</v>
-    </oc>
-    <nc r="D12">
-      <v>3</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="66" sId="1">
-    <nc r="D13">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="67" sId="1">
-    <nc r="D14">
-      <v>4</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="68" sId="1">
-    <nc r="D26">
-      <v>10</v>
-    </nc>
-  </rcc>
-  <rcc rId="69" sId="1">
-    <nc r="D27">
-      <v>10</v>
-    </nc>
-  </rcc>
-  <rcc rId="70" sId="1">
-    <nc r="D28">
-      <v>5</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="1" sheetId="1" source="C11" destination="C19" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C19" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="2" sheetId="1" source="C8:C10" destination="C9:C11" sourceSheetId="1"/>
-  <rm rId="3" sheetId="1" source="C19" destination="C8" sourceSheetId="1"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="71" sId="1">
-    <oc r="D28">
-      <v>5</v>
-    </oc>
-    <nc r="D28">
-      <v>6</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="72" sId="1">
-    <oc r="D28">
-      <v>6</v>
-    </oc>
-    <nc r="D28">
+  <rcc rId="278" sId="1">
+    <oc r="D15">
+      <v>3</v>
+    </oc>
+    <nc r="D15">
       <v>4</v>
     </nc>
   </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="73" sheetId="1" source="F14" destination="F16" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="F16" start="0" length="0">
-      <dxf/>
-    </rfmt>
-  </rm>
-  <rcc rId="74" sId="1">
-    <oc r="B34" t="inlineStr">
-      <is>
-        <t>das war eig. Bis MR1 geplant:</t>
-      </is>
-    </oc>
-    <nc r="B34"/>
-  </rcc>
-  <rcc rId="75" sId="1">
-    <oc r="C35" t="inlineStr">
-      <is>
-        <t>Jetzt ca. ein Sprint bis zum MR 1</t>
-      </is>
-    </oc>
-    <nc r="C35"/>
-  </rcc>
-  <rcc rId="76" sId="1">
-    <oc r="B36" t="inlineStr">
-      <is>
-        <t>da wird voraussichtlich gemacht:</t>
-      </is>
-    </oc>
-    <nc r="B36"/>
-  </rcc>
-  <rcc rId="77" sId="1">
-    <oc r="B37" t="inlineStr">
-      <is>
-        <t>.) Kunde anlegen</t>
-      </is>
-    </oc>
-    <nc r="B37"/>
-  </rcc>
-  <rcc rId="78" sId="1">
-    <oc r="B38" t="inlineStr">
-      <is>
-        <t>.) Kunde bearbeiten (beides mit UI - nicht vergessen auf auslagern der Texte im UI)</t>
-      </is>
-    </oc>
-    <nc r="B38"/>
-  </rcc>
-  <rcc rId="79" sId="1">
-    <oc r="B39" t="inlineStr">
-      <is>
-        <t>.) Kunden-Demo-Demo-Daten erstellen</t>
-      </is>
-    </oc>
-    <nc r="B39"/>
-  </rcc>
-  <rcc rId="80" sId="1">
-    <oc r="B40" t="inlineStr">
-      <is>
-        <t>.) Demo-Daten für Veranstaltungen erstellen</t>
-      </is>
-    </oc>
-    <nc r="B40"/>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="81" sId="1">
-    <nc r="F5" t="inlineStr">
-      <is>
-        <t>Storypoints pro Sprint:</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="82" sId="1">
-    <nc r="F6">
-      <v>40</v>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="F5:F6">
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="F5" start="0" length="0">
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F6" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F6">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="83" sId="1">
-    <oc r="F6">
-      <v>40</v>
-    </oc>
-    <nc r="F6">
-      <v>50</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="84" sheetId="1" source="F3" destination="F9" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="F9" start="0" length="0">
-      <dxf/>
-    </rfmt>
-  </rm>
-  <rcc rId="85" sId="1">
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>Calvin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="86" sId="1">
-    <nc r="E6" t="inlineStr">
-      <is>
-        <t>Calvin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="87" sId="1">
-    <nc r="E7" t="inlineStr">
-      <is>
-        <t>Benni</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="88" sId="1">
-    <nc r="E9" t="inlineStr">
-      <is>
-        <t>Calvin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="89" sId="1">
-    <nc r="E8" t="inlineStr">
-      <is>
-        <t>Alex</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="E5:E28">
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="E5:E28">
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="E5:E28">
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="E5:E28">
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="E5:E28">
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="C14:E14" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="90" sId="1">
-    <nc r="B14" t="inlineStr">
-      <is>
-        <t>1. Sprint bis hierher</t>
-      </is>
-    </nc>
-  </rcc>
-  <rm rId="91" sheetId="1" source="B14" destination="A14" sourceSheetId="1"/>
-  <rcc rId="92" sId="1">
-    <nc r="E13" t="inlineStr">
-      <is>
-        <t>Martin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="93" sId="1">
-    <nc r="E14" t="inlineStr">
-      <is>
-        <t>Martin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="94" sId="1">
-    <nc r="E4" t="inlineStr">
-      <is>
-        <t>Verantwortlicher:</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="95" sId="1">
-    <nc r="E11" t="inlineStr">
-      <is>
-        <t>Christopher</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="96" sId="1">
-    <nc r="E12" t="inlineStr">
-      <is>
-        <t>Christopher</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="97" sId="1">
-    <nc r="E10" t="inlineStr">
-      <is>
-        <t>Christopher</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="C12:C21" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C12:C21">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-      </border>
-    </dxf>
-  </rfmt>
-  <rm rId="4" sheetId="1" source="F15" destination="C18" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C18" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="5" sheetId="1" source="C18" destination="C15" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C15" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="6" sheetId="1" source="F12" destination="C16" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C16" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="7" sheetId="1" source="F13" destination="C17" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C17" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="8" sheetId="1" source="F14" destination="C18" sourceSheetId="1"/>
-  <rm rId="9" sheetId="1" source="F11" destination="C19" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C19" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="10" sheetId="1" source="F10" destination="C20" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C20" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rfmt sheetId="1" sqref="C14:C24" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C14:C24">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="E4" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D4" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="E4" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="F5:F6" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5:F6" start="0" length="0">
-    <dxf>
-      <border>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F6" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F5" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rrc rId="98" sId="1" ref="F1:F1048576" action="insertCol"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
 </revisions>
 </file>
 
@@ -2574,35 +1646,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="11" sheetId="1" source="C18" destination="C24" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C24" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="12" sheetId="1" source="C16:C17" destination="C17:C18" sourceSheetId="1"/>
-  <rm rId="13" sheetId="1" source="C24" destination="C16" sourceSheetId="1"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="129" sId="1">
@@ -3007,281 +2050,6 @@
       </is>
     </nc>
   </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="14" sheetId="1" source="C19" destination="C23" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C23" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="15" sheetId="1" source="C18" destination="C19" sourceSheetId="1"/>
-  <rm rId="16" sheetId="1" source="C23" destination="C18" sourceSheetId="1"/>
-  <rfmt sheetId="1" sqref="C15:C24" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C15:C24">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-      </border>
-    </dxf>
-  </rfmt>
-  <rm rId="17" sheetId="1" source="F8" destination="C21" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C21" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rfmt sheetId="1" sqref="C20:C21" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C20:C21">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C20:C22">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="18" sId="1">
-    <oc r="F3" t="inlineStr">
-      <is>
-        <t>noch reihen - Base Use Stories</t>
-      </is>
-    </oc>
-    <nc r="F3"/>
-  </rcc>
-  <rcc rId="19" sId="1">
-    <oc r="F5" t="inlineStr">
-      <is>
-        <t>Kunden</t>
-      </is>
-    </oc>
-    <nc r="F5"/>
-  </rcc>
-  <rcc rId="20" sId="1">
-    <oc r="F9" t="inlineStr">
-      <is>
-        <t>Veranstaltungen</t>
-      </is>
-    </oc>
-    <nc r="F9"/>
-  </rcc>
-  <rcc rId="21" sId="1">
-    <oc r="F16" t="inlineStr">
-      <is>
-        <t>Tickets:</t>
-      </is>
-    </oc>
-    <nc r="F16"/>
-  </rcc>
-  <rcc rId="22" sId="1">
-    <oc r="F23" t="inlineStr">
-      <is>
-        <t>Rechnungsdruck</t>
-      </is>
-    </oc>
-    <nc r="F23"/>
-  </rcc>
-  <rfmt sheetId="1" sqref="F2:F24" start="0" length="0">
-    <dxf>
-      <border>
-        <left/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F2:F24" start="0" length="0">
-    <dxf>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rm rId="23" sheetId="1" source="F10:F12" destination="F12:F14" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="F13" start="0" length="0">
-      <dxf/>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F14" start="0" length="0">
-      <dxf/>
-    </rfmt>
-  </rm>
-  <rm rId="24" sheetId="1" source="F34" destination="C23" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C23" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="25" sheetId="1" source="F35" destination="C24" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C24" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rm rId="26" sheetId="1" source="F36" destination="C25" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C25" start="0" length="0">
-      <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rrc rId="27" sId="1" ref="A25:XFD25" action="insertRow"/>
-  <rm rId="28" sheetId="1" source="C24" destination="C25" sourceSheetId="1"/>
-  <rm rId="29" sheetId="1" source="C26" destination="C24" sourceSheetId="1"/>
-  <rrc rId="30" sId="1" ref="A26:XFD26" action="insertRow"/>
-  <rrc rId="31" sId="1" ref="A26:XFD26" action="insertRow"/>
-  <rcc rId="32" sId="1">
-    <oc r="F36" t="inlineStr">
-      <is>
-        <t>Benutzerverwaltung</t>
-      </is>
-    </oc>
-    <nc r="F36"/>
-  </rcc>
-  <rfmt sheetId="1" sqref="F36" start="0" length="0">
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C20:C28" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C28:D28" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
 </revisions>
 </file>
 
@@ -3732,84 +2500,6 @@
       <font>
         <color rgb="FF00B050"/>
       </font>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="1" sqref="C22" start="0" length="0">
-    <dxf>
-      <border>
-        <left/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C22:D22" start="0" length="0">
-    <dxf>
-      <border>
-        <top/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D22" start="0" length="0">
-    <dxf>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C22:D22" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C22:D22">
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C19:D19" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C21:D21" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C23:D23" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C24:D24" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </rfmt>
 </revisions>
@@ -4578,11 +3268,247 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog68.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="33" sheetId="1" source="F33" destination="C27" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C27" start="0" length="0">
+  <rcc rId="227" sId="1">
+    <oc r="D15">
+      <v>4</v>
+    </oc>
+    <nc r="D15">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C21:D21" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="228" sId="1">
+    <oc r="D18">
+      <v>6</v>
+    </oc>
+    <nc r="D18">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcc rId="229" sId="1">
+    <oc r="D20">
+      <v>8</v>
+    </oc>
+    <nc r="D20">
+      <v>6</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog69.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="A21" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="230" sId="1">
+    <nc r="A21" t="inlineStr">
+      <is>
+        <t>2. Sprint bis hierher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="A21:B21" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A21:B21" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog70.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="231" sId="1">
+    <oc r="C29" t="inlineStr">
+      <is>
+        <t>Übersicht alles Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+      </is>
+    </oc>
+    <nc r="C29" t="inlineStr">
+      <is>
+        <t>Stornierungen und PDF neu drucken</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="232" sId="1">
+    <oc r="D29">
+      <v>4</v>
+    </oc>
+    <nc r="D29">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="233" sId="1">
+    <oc r="D30">
+      <v>3</v>
+    </oc>
+    <nc r="D30">
+      <v>5</v>
+    </nc>
+  </rcc>
+  <rcc rId="234" sId="1">
+    <oc r="D31">
+      <v>3</v>
+    </oc>
+    <nc r="D31">
+      <v>4</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog71.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="235" sId="1">
+    <oc r="D35">
+      <v>2</v>
+    </oc>
+    <nc r="D35">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog72.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C15:D15" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E15" start="0" length="2147483647">
+    <dxf>
+      <font/>
+    </dxf>
+  </rfmt>
+  <rcc rId="236" sId="1">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>Martin / Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="237" sId="1">
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>Martin / Calvin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="238" sId="1">
+    <nc r="E16" t="inlineStr">
+      <is>
+        <t>Alex / Benni</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E16" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E13:E14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E17:E21" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C17:E17" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="239" sId="1">
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>was soll der Punkt - ist doch das selbe wie oben oder?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="240" sId="1" ref="A22:XFD22" action="insertRow"/>
+  <rm rId="241" sheetId="1" source="C30:D30" destination="C22:D22" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="C22" start="0" length="0">
       <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
         <border outline="0">
           <left style="thin">
             <color indexed="64"/>
@@ -4590,39 +3516,233 @@
           <right style="thin">
             <color indexed="64"/>
           </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D22" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
         </border>
       </dxf>
     </rfmt>
   </rm>
-  <rm rId="34" sheetId="1" source="F34" destination="C28" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C28" start="0" length="0">
+  <rrc rId="242" sId="1" ref="A30:XFD30" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A30:XFD30" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="E30" start="0" length="0">
       <dxf>
-        <border outline="0">
-          <left style="thin">
-            <color indexed="64"/>
-          </left>
-          <right style="thin">
-            <color indexed="64"/>
-          </right>
-          <top style="thin">
-            <color indexed="64"/>
-          </top>
-          <bottom style="thin">
-            <color indexed="64"/>
-          </bottom>
-        </border>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F30" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G30" start="0" length="0">
+      <dxf/>
+    </rfmt>
+  </rrc>
+  <rfmt sheetId="1" sqref="C22:D22" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C22:D22">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C22:D22" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rm rId="243" sheetId="1" source="A21" destination="A22" sourceSheetId="1">
+    <rfmt sheetId="1" sqref="A22" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="5"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
       </dxf>
     </rfmt>
   </rm>
-  <rm rId="35" sheetId="1" source="C27:C28" destination="C26:C27" sourceSheetId="1">
-    <rfmt sheetId="1" sqref="C26" start="0" length="0">
-      <dxf>
+  <rcc rId="244" sId="1">
+    <oc r="D22">
+      <v>2</v>
+    </oc>
+    <nc r="D22">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="245" sId="1">
+    <nc r="E22" t="inlineStr">
+      <is>
+        <t>notwendig als eigener Punkt?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="246" sId="1">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>notwendig als eigener Punkt??</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E22" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C22:D22" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog73.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C8:E11" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C13:E14" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A22" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C15:E19" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="247" sId="1">
+    <oc r="D18">
+      <v>4</v>
+    </oc>
+    <nc r="D18">
+      <v>6</v>
+    </nc>
+  </rcc>
+  <rcc rId="248" sId="1">
+    <oc r="D20">
+      <v>6</v>
+    </oc>
+    <nc r="D20">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rm rId="249" sheetId="1" source="A22" destination="A20" sourceSheetId="1"/>
+  <rfmt sheetId="1" sqref="C20:D20" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C20:D20" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="250" sId="1">
+    <oc r="E22" t="inlineStr">
+      <is>
+        <t>notwendig als eigener Punkt?</t>
+      </is>
+    </oc>
+    <nc r="E22"/>
+  </rcc>
+  <rfmt sheetId="1" sqref="C22:D23">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C22:D22" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rrc rId="251" sId="1" ref="A29:XFD29" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A29:XFD29" start="0" length="0"/>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C29" t="inlineStr">
+        <is>
+          <t>Mehrsprachigkeit - laufend</t>
+        </is>
+      </nc>
+      <ndxf>
         <border outline="0">
           <left style="thin">
             <color indexed="64"/>
@@ -4637,129 +3757,436 @@
             <color indexed="64"/>
           </bottom>
         </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="D29">
+        <v>5</v>
+      </nc>
+      <ndxf>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="E29" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
       </dxf>
     </rfmt>
-  </rm>
-  <rm rId="36" sheetId="1" source="C26:C27" destination="C27:C28" sourceSheetId="1"/>
-  <rm rId="37" sheetId="1" source="F35" destination="C26" sourceSheetId="1"/>
-  <rfmt sheetId="1" sqref="C24:C28" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="C28:D28" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="38" sId="1">
-    <oc r="F31" t="inlineStr">
-      <is>
-        <t>erweiterte User-Stories:</t>
-      </is>
-    </oc>
-    <nc r="F31"/>
-  </rcc>
-  <rcc rId="39" sId="1">
-    <oc r="F32" t="inlineStr">
-      <is>
-        <t>Zahlungsabwicklung</t>
-      </is>
-    </oc>
-    <nc r="F32"/>
-  </rcc>
-  <rfmt sheetId="1" sqref="F30:F34" start="0" length="0">
-    <dxf>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="40" sheetId="1" source="C26" destination="C29" sourceSheetId="1"/>
-  <rm rId="41" sheetId="1" source="C27:C29" destination="C26:C28" sourceSheetId="1"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
-  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="42" sId="1" ref="A32:XFD32" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A32:XFD32" start="0" length="0"/>
-    <rfmt sheetId="1" sqref="E32" start="0" length="0">
-      <dxf/>
+    <rfmt sheetId="1" sqref="F29" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
     </rfmt>
-    <rfmt sheetId="1" sqref="F32" start="0" length="0">
+    <rfmt sheetId="1" sqref="G29" start="0" length="0">
       <dxf/>
     </rfmt>
   </rrc>
-  <rrc rId="43" sId="1" ref="A32:XFD32" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A32:XFD32" start="0" length="0"/>
-    <rfmt sheetId="1" sqref="E32" start="0" length="0">
-      <dxf/>
+  <rfmt sheetId="1" sqref="C19:D19" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C21:D21" start="0" length="0">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C21:D22">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="252" sId="1">
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t>2. Sprint bis hierher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="253" sId="1">
+    <oc r="A20" t="inlineStr">
+      <is>
+        <t>2. Sprint bis hierher</t>
+      </is>
+    </oc>
+    <nc r="A20"/>
+  </rcc>
+  <rcc rId="254" sId="1">
+    <nc r="E18" t="inlineStr">
+      <is>
+        <t>Calvin/Christopfer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="255" sId="1">
+    <nc r="E19" t="inlineStr">
+      <is>
+        <t>Calvin/Christopfer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="256" sId="1" odxf="1" dxf="1">
+    <oc r="E17" t="inlineStr">
+      <is>
+        <t>was soll der Punkt - ist doch das selbe wie oben oder?</t>
+      </is>
+    </oc>
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>Calvin/Christopfer</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment horizontal="left" vertical="top" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="257" sId="1" odxf="1" dxf="1">
+    <oc r="E15" t="inlineStr">
+      <is>
+        <t>notwendig als eigener Punkt??</t>
+      </is>
+    </oc>
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>Calvin/Christopfer</t>
+      </is>
+    </nc>
+    <ndxf/>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog74.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="258" sId="1" ref="A22:XFD22" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A22:XFD22" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="B22" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="5"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </dxf>
     </rfmt>
-    <rfmt sheetId="1" sqref="F32" start="0" length="0">
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="C22" t="inlineStr">
+        <is>
+          <t>Stornierungen und PDF neu drucken</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment vertical="top" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="D22">
+        <v>1</v>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color auto="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="center" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="64"/>
+          </left>
+          <right style="thin">
+            <color indexed="64"/>
+          </right>
+          <top style="thin">
+            <color indexed="64"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="64"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="E22" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color rgb="FFFF0000"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F22" start="0" length="0">
+      <dxf>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G22" start="0" length="0">
       <dxf/>
     </rfmt>
   </rrc>
-  <rrc rId="44" sId="1" ref="A32:XFD32" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A32:XFD32" start="0" length="0"/>
-    <rfmt sheetId="1" sqref="E32" start="0" length="0">
-      <dxf/>
-    </rfmt>
-    <rfmt sheetId="1" sqref="F32" start="0" length="0">
-      <dxf/>
-    </rfmt>
-  </rrc>
-  <rrc rId="45" sId="1" ref="A32:XFD32" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A32:XFD32" start="0" length="0"/>
-  </rrc>
-  <rrc rId="46" sId="1" ref="A32:XFD32" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A32:XFD32" start="0" length="0"/>
-    <rfmt sheetId="1" sqref="F32" start="0" length="0">
-      <dxf/>
-    </rfmt>
-  </rrc>
-  <rcc rId="47" sId="1">
-    <nc r="D5">
+  <rcc rId="259" sId="1">
+    <oc r="D29">
+      <v>4</v>
+    </oc>
+    <nc r="D29">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcc rId="260" sId="1">
+    <oc r="D28">
+      <v>5</v>
+    </oc>
+    <nc r="D28">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog75.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="261" sId="1">
+    <nc r="A30" t="inlineStr">
+      <is>
+        <t>3. Sprint bis hierher</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="E21" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rcc rId="262" sId="1">
+    <nc r="E20" t="inlineStr">
+      <is>
+        <t>Christopher?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="263" sId="1">
+    <nc r="E21" t="inlineStr">
+      <is>
+        <t>Christopher?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C20:D20" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog76.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="264" sId="1">
+    <nc r="E22" t="inlineStr">
+      <is>
+        <t>Alex/Benni ?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="265" sId="1">
+    <nc r="E23" t="inlineStr">
+      <is>
+        <t>Alex/Benni ?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="266" sId="1">
+    <nc r="E24" t="inlineStr">
+      <is>
+        <t>Alex/Benni ?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="267" sId="1">
+    <nc r="E25" t="inlineStr">
+      <is>
+        <t>Alex/Benni ?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="268" sId="1">
+    <nc r="E26" t="inlineStr">
+      <is>
+        <t>Alex/Benni ?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="269" sId="1">
+    <nc r="E28" t="inlineStr">
+      <is>
+        <t>Calvin/Martin?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="270" sId="1">
+    <nc r="E29" t="inlineStr">
+      <is>
+        <t>Calvin/Martin?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="271" sId="1">
+    <nc r="E30" t="inlineStr">
+      <is>
+        <t>Calvin/Martin?</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog77.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="272" sId="1" ref="A28:XFD28" action="insertRow"/>
+  <rcc rId="273" sId="1">
+    <nc r="D28">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="C28:E28" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="274" sId="1">
+    <nc r="E28" t="inlineStr">
+      <is>
+        <t>ist doch bereits erledigt oder?</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="275" sId="1" odxf="1" dxf="1">
+    <nc r="C28" t="inlineStr">
+      <is>
+        <t>Übersicht aller Rechnungen/Reservierungen
+Stornierungen und PDF neu drucken</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog78.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="276" sId="1">
+    <oc r="D31">
+      <v>1</v>
+    </oc>
+    <nc r="D31">
       <v>2</v>
     </nc>
   </rcc>
-  <rfmt sheetId="1" sqref="D5:D28">
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="D5:D28">
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="48" sId="1">
-    <nc r="D6">
-      <v>2</v>
-    </nc>
-  </rcc>
+  <rcc rId="277" sId="1">
+    <oc r="D28">
+      <v>4</v>
+    </oc>
+    <nc r="D28">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog79.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C31:D31" start="0" length="0">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog80.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="E20:E21" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
 </revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{6D67104E-9692-4EB5-A708-D75F28C04361}" name="Microsoft" id="-471496629" dateTime="2017-05-10T21:54:50"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5025,17 +4452,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
@@ -5045,10 +4472,10 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
@@ -5063,263 +4490,289 @@
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <v>4</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>43</v>
+      <c r="E5" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="14" t="s">
-        <v>24</v>
+      <c r="G5" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>3</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>43</v>
+      <c r="E6" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="30">
+      <c r="G6" s="26">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="16">
         <v>4</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>34</v>
+      <c r="E7" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="27">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="16">
         <v>14</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="E8" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="28">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="35">
         <v>5</v>
       </c>
-      <c r="E9" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="E9" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="29">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="37">
         <v>3</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="E10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="27">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="E11" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="40">
+      <c r="A12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="29">
         <v>4</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="E12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-      <c r="C13" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="27">
+      <c r="B13" s="23"/>
+      <c r="C13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="16">
         <v>3</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="E13" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
-      <c r="C14" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="27">
+      <c r="B14" s="23"/>
+      <c r="C14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="16">
         <v>3</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="E14" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="16">
         <v>4</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="E15" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="27">
+      <c r="C16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="16">
         <v>10</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="23"/>
+      <c r="E16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="37">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="40">
         <v>3</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="E17" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="16">
         <v>6</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="24"/>
+      <c r="E18" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="22"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="26" t="s">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="29">
         <v>3</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="26" t="s">
+      <c r="A20" s="23"/>
+      <c r="C20" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="42">
         <v>8</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="25">
         <v>4</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="13"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="8">
         <v>5</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
@@ -5330,7 +4783,9 @@
       <c r="D23" s="8">
         <v>1</v>
       </c>
-      <c r="E23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
@@ -5341,7 +4796,9 @@
       <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
@@ -5352,7 +4809,9 @@
       <c r="D25" s="9">
         <v>1</v>
       </c>
-      <c r="E25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
@@ -5363,7 +4822,9 @@
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
@@ -5378,74 +4839,85 @@
       <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="8">
-        <v>5</v>
-      </c>
-      <c r="E28" s="11"/>
+    <row r="28" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="33">
+        <v>3</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>51</v>
+      </c>
       <c r="F28" s="11"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C29" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="27">
-        <v>4</v>
-      </c>
-      <c r="E29" s="11"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="25">
+        <v>3</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="F29" s="11"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="27">
+      <c r="C30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="25">
         <v>3</v>
       </c>
-      <c r="E30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="F30" s="11"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="27">
-        <v>3</v>
-      </c>
-      <c r="E31" s="11"/>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="44">
+        <v>2</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="F31" s="11"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="27">
-        <v>1</v>
-      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="3"/>
-      <c r="D33" s="10"/>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="8">
+        <v>4</v>
+      </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -5453,7 +4925,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="8">
         <v>2</v>
@@ -5464,10 +4936,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D36" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -5475,48 +4947,40 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D37" s="8">
         <v>10</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="8">
-        <v>4</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" s="3"/>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="6"/>
+    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
@@ -5530,13 +4994,10 @@
     <row r="49" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
     </row>
-    <row r="50" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="5"/>
-    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5545,13 +5006,13 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
-      <selection activeCell="G7" sqref="G7"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="G16" sqref="G16"/>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" topLeftCell="A7">
+      <selection activeCell="F22" sqref="F22"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>

</xml_diff>

<commit_message>
added final formatted documents
</commit_message>
<xml_diff>
--- a/documents/Product Backlog inkl Bewertung.xlsx
+++ b/documents/Product Backlog inkl Bewertung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Martin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Microsoft - Persönliche Ansicht" guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" mergeInterval="0" personalView="1" xWindow="2173" windowWidth="960" windowHeight="1040" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
     <customWorkbookView name="Martin Klampfer - Persönliche Ansicht" guid="{B81880CA-6D53-4284-8FE7-C2592317081E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-11" yWindow="-11" windowWidth="2182" windowHeight="1402" activeSheetId="1"/>
-    <customWorkbookView name="Alex - Persönliche Ansicht" guid="{C5B156C7-D343-4698-A97F-B19105873C1E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="850" activeSheetId="1"/>
-    <customWorkbookView name="Benni - Persönliche Ansicht" guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -89,9 +89,6 @@
     <t>1. Sprint bis hierher</t>
   </si>
   <si>
-    <t>Verantwortlicher:</t>
-  </si>
-  <si>
     <t>Christopher</t>
   </si>
   <si>
@@ -172,13 +169,16 @@
   </si>
   <si>
     <t>Calvin/Martin/Alex/Benni</t>
+  </si>
+  <si>
+    <t>Verantwortliche(r):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,13 +203,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -393,13 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -418,35 +404,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,15 +417,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,7 +473,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7A8E6BA9-E5EF-44D4-8EF2-9D05F194A3D1}" diskRevisions="1" revisionId="312" version="41">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2DB8D3E1-FCBE-4F95-B659-E413D31831B8}" diskRevisions="1" revisionId="313" version="43">
   <header guid="{B7332BE5-164E-4387-8C18-B3206B81A70E}" dateTime="2017-05-10T22:15:45" maxSheetId="2" userName="Microsoft" r:id="rId73" minRId="227" maxRId="229">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -569,7 +559,31 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{80BB696B-C6F1-47F6-BD18-2DA35100FD04}" dateTime="2017-06-20T10:04:12" maxSheetId="2" userName="Microsoft" r:id="rId90">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2DB8D3E1-FCBE-4F95-B659-E413D31831B8}" dateTime="2017-06-20T10:04:21" maxSheetId="2" userName="Microsoft" r:id="rId91" minRId="313">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C5:E30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="delete"/>
+  <rcv guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1409,6 +1423,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="313" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <t>Verantwortlicher:</t>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <t>Verantwortliche(r):</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog68.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="227" sId="1">
@@ -2324,9 +2355,10 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{6D67104E-9692-4EB5-A708-D75F28C04361}" name="Microsoft" id="-471496629" dateTime="2017-05-10T21:54:50"/>
+  <userInfo guid="{2DB8D3E1-FCBE-4F95-B659-E413D31831B8}" name="Microsoft" id="-471499721" dateTime="2017-06-20T10:03:56"/>
 </users>
 </file>
 
@@ -2596,7 +2628,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,10 +2645,10 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="4"/>
       <c r="G2" s="3"/>
     </row>
@@ -2631,21 +2663,21 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="25">
         <v>4</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>35</v>
+      <c r="E5" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9" t="s">
@@ -2654,291 +2686,291 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="27">
         <v>3</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>35</v>
+      <c r="E6" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="21">
+      <c r="G6" s="18">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="27">
         <v>4</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>26</v>
+      <c r="E7" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="27">
         <v>14</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="29">
         <v>5</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+        <v>35</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="11" t="s">
-        <v>33</v>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="31">
         <v>3</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="E10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="27">
         <v>3</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="E11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="33">
+        <v>4</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="27">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="27">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="27">
+        <v>3</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="24">
-        <v>4</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="13">
+      <c r="D16" s="27">
+        <v>10</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="35">
         <v>3</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E17" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="13">
-        <v>3</v>
-      </c>
-      <c r="E14" s="25" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="27">
+        <v>6</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="13">
-        <v>3</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="13">
-        <v>10</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="18"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="33">
-        <v>3</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="13">
-        <v>6</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="33">
         <v>3</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>40</v>
+      <c r="E19" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="17"/>
       <c r="C20" s="36" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="37">
         <v>8</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>20</v>
+      <c r="E20" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="27">
         <v>4</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>20</v>
+      <c r="E21" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="27">
         <v>5</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>42</v>
+      <c r="E22" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="27">
         <v>2</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>42</v>
+      <c r="E23" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="27">
         <v>2</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>42</v>
+      <c r="E24" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="3"/>
@@ -2950,76 +2982,76 @@
       <c r="D25" s="39">
         <v>2</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>42</v>
+      <c r="E25" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="27">
         <v>2</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>42</v>
+      <c r="E26" s="26" t="s">
+        <v>41</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="27">
         <v>7</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>43</v>
+      <c r="E27" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="13">
+      <c r="C28" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="27">
         <v>3</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>35</v>
+      <c r="E28" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="13">
+      <c r="C29" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="27">
         <v>3</v>
       </c>
-      <c r="E29" s="22" t="s">
-        <v>35</v>
+      <c r="E29" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="24">
+        <v>40</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="33">
         <v>2</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>35</v>
+      <c r="E30" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="3"/>
@@ -3040,26 +3072,26 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="40">
+        <v>43</v>
+      </c>
+      <c r="D33" s="21">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="21">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
         <v>45</v>
-      </c>
-      <c r="D34" s="40">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>46</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="3"/>
@@ -3092,13 +3124,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}">
-      <selection activeCell="E38" sqref="E38"/>
+    <customSheetView guid="{008EB867-0C7F-45CC-AC1A-B47163F994FF}" topLeftCell="A3">
+      <selection activeCell="G19" sqref="G19"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
-      <selection activeCell="G7" sqref="G7"/>
+    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -3107,8 +3139,8 @@
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3096D4FF-FF3B-428E-9265-C3A523BB5404}" topLeftCell="A4">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{B81880CA-6D53-4284-8FE7-C2592317081E}">
+      <selection activeCell="G7" sqref="G7"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>

</xml_diff>